<commit_message>
ADD: microcolony suspension colony size setting
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMXCMX.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMXCMX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A812433-CB47-4D49-8A40-E58DF08F6EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A674F5F-0E9D-407A-AD6D-F32455A5F8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -38,6 +38,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -214,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="292">
   <si>
     <t>AOB/AOA</t>
   </si>
@@ -1463,58 +1464,64 @@
     <t>This cell contains the units of the value that should be filled in. Don’t change the contents of these cells, but rather make sure that the filled in value is in these units</t>
   </si>
   <si>
-    <t>Suspension: how many bacteria start in the suspension</t>
-  </si>
-  <si>
     <t>Starting number of bacteria (granule)</t>
   </si>
   <si>
-    <t>Starting number of bacteria (suspension)</t>
-  </si>
-  <si>
     <t>CALCULATED: approximated number of bacteria in the starting granule, based on optimal packing of bacteria in circle. Will be slightly lower in reality</t>
   </si>
   <si>
     <t>Fill in the yields &amp; electron donor molecules for each species. If the maintenance and growth rate are to be set, fill them in as well. If these are to be calculated on the fly, leave blank or fill in 'NA'. The formula for the maintenance and growth rate should manually be added to the calculate_max_growth_rate_and_maint.m script</t>
   </si>
   <si>
-    <t>Starting bio-aggregate in the system</t>
-  </si>
-  <si>
     <t>NOB</t>
   </si>
   <si>
     <t>Yield C/N</t>
   </si>
   <si>
+    <t>Average expected granule radius</t>
+  </si>
+  <si>
+    <t>density granule</t>
+  </si>
+  <si>
+    <t>density reactor</t>
+  </si>
+  <si>
+    <t>g/L</t>
+  </si>
+  <si>
+    <t>CALCULATED Representative volume of the reactor that is modelled in the simulation domain. Calculated using the average expected granule radius and the density of biomass in the reactor and the density per granule</t>
+  </si>
+  <si>
+    <t>Average expected radius of all granules</t>
+  </si>
+  <si>
+    <t>How much biomass (at most) is in the reactor</t>
+  </si>
+  <si>
+    <t>How dense are the granules</t>
+  </si>
+  <si>
+    <t>Starting bio-aggregate in the system (mature granule =&gt; AMX in center of granule)</t>
+  </si>
+  <si>
     <t>none</t>
   </si>
   <si>
-    <t>Average expected granule radius</t>
-  </si>
-  <si>
-    <t>density granule</t>
-  </si>
-  <si>
-    <t>density reactor</t>
-  </si>
-  <si>
-    <t>g/L</t>
-  </si>
-  <si>
-    <t>CALCULATED Representative volume of the reactor that is modelled in the simulation domain. Calculated using the average expected granule radius and the density of biomass in the reactor and the density per granule</t>
-  </si>
-  <si>
-    <t>Average expected radius of all granules</t>
-  </si>
-  <si>
-    <t>How much biomass (at most) is in the reactor</t>
-  </si>
-  <si>
-    <t>How dense are the granules</t>
-  </si>
-  <si>
-    <t>granule</t>
+    <t>suspension</t>
+  </si>
+  <si>
+    <t>Starting number of microcolonies (suspension)</t>
+  </si>
+  <si>
+    <t>Suspension: how many microcolonies start in the suspension</t>
+  </si>
+  <si>
+    <t>Suspension: how many bacteria start in the suspension per microcolony</t>
+  </si>
+  <si>
+    <t>Starting number of bacteria per microcolony (suspension)</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1900,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="83">
+  <borders count="86">
     <border>
       <left/>
       <right/>
@@ -2955,6 +2962,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2970,7 +3012,7 @@
     <xf numFmtId="0" fontId="35" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
@@ -3313,9 +3355,6 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="10" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="11" borderId="54" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="11" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3569,9 +3608,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="50" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="37" fillId="0" borderId="22" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3590,6 +3626,9 @@
     </xf>
     <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="11" borderId="54" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3667,6 +3706,18 @@
     </xf>
     <xf numFmtId="0" fontId="24" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="83" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -3683,7 +3734,87 @@
     <cellStyle name="Percent" xfId="8" builtinId="5"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="87">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
@@ -3953,56 +4084,6 @@
         <i/>
         <color theme="0" tint="-0.34998626667073579"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4588,71 +4669,71 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A9" s="227" t="s">
+      <c r="A9" s="226" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="228" t="s">
+      <c r="A10" s="227" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="226" t="s">
+      <c r="A11" s="225" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="225" t="s">
+      <c r="A12" s="224" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="221" t="s">
+      <c r="A13" s="220" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="220" t="s">
+      <c r="A14" s="219" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="222" t="s">
+      <c r="A15" s="221" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="223" t="s">
+      <c r="A16" s="222" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="224" t="s">
+      <c r="A17" s="223" t="s">
         <v>270</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="83" priority="6">
+    <cfRule type="expression" dxfId="86" priority="6">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="82" priority="4" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="85" priority="4" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="5" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="84" priority="5" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="80" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="79" priority="1">
+    <cfRule type="expression" dxfId="82" priority="1">
       <formula>$B$11&lt;&gt;"naive"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4666,7 +4747,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4684,12 +4765,13 @@
         <v>74</v>
       </c>
       <c r="B1" s="131">
-        <v>9.9999999999999995E-7</v>
+        <f>500*10^(-6)</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="258" t="s">
+      <c r="D1" s="257" t="s">
         <v>231</v>
       </c>
       <c r="E1" s="69"/>
@@ -4701,12 +4783,13 @@
         <v>75</v>
       </c>
       <c r="B2" s="131">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" ref="B2:B3" si="0">500*10^(-6)</f>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="258"/>
+      <c r="D2" s="257"/>
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
@@ -4716,12 +4799,13 @@
         <v>80</v>
       </c>
       <c r="B3" s="131">
-        <v>9.9999999999999995E-7</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="258"/>
+      <c r="D3" s="257"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
@@ -4737,7 +4821,7 @@
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="258"/>
+      <c r="D4" s="257"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
@@ -4752,7 +4836,7 @@
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="258"/>
+      <c r="D5" s="257"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
@@ -4763,41 +4847,41 @@
       </c>
       <c r="B6" s="135">
         <f>B1/2</f>
-        <v>4.9999999999999998E-7</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="C6" s="126" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="258"/>
+      <c r="D6" s="257"/>
       <c r="E6" s="69"/>
       <c r="F6" s="69"/>
       <c r="G6" s="69"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="150" t="s">
+      <c r="A7" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="151">
+      <c r="B7" s="150">
         <v>1E-10</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="258"/>
+      <c r="D7" s="257"/>
       <c r="E7" s="69"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="146"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="145"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="69"/>
-      <c r="F8" s="147"/>
-      <c r="G8" s="148"/>
-      <c r="H8" s="149"/>
-      <c r="I8" s="147"/>
-      <c r="J8" s="146"/>
+      <c r="F8" s="146"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="148"/>
+      <c r="I8" s="146"/>
+      <c r="J8" s="145"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="69"/>
@@ -4824,7 +4908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4838,25 +4922,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="161" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="162" t="s">
+      <c r="C1" s="161" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="163" t="s">
+      <c r="D1" s="162" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="162" t="s">
+      <c r="E1" s="161" t="s">
         <v>235</v>
       </c>
-      <c r="F1" s="163" t="s">
+      <c r="F1" s="162" t="s">
         <v>236</v>
       </c>
-      <c r="G1" s="163" t="s">
+      <c r="G1" s="162" t="s">
         <v>250</v>
       </c>
     </row>
@@ -4864,28 +4948,28 @@
       <c r="A2" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="171">
+      <c r="C2" s="170">
         <v>-79.37</v>
       </c>
-      <c r="D2" s="171">
+      <c r="D2" s="170">
         <v>-26.57</v>
       </c>
-      <c r="E2" s="171" t="s">
+      <c r="E2" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="171" t="s">
+      <c r="F2" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="168">
+      <c r="G2" s="167">
         <v>3</v>
       </c>
-      <c r="H2" s="164" t="s">
+      <c r="H2" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="258" t="s">
+      <c r="I2" s="257" t="s">
         <v>251</v>
       </c>
     </row>
@@ -4893,262 +4977,262 @@
       <c r="A3" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="171">
+      <c r="C3" s="170">
         <v>-50.6</v>
       </c>
-      <c r="D3" s="171">
+      <c r="D3" s="170">
         <v>-32.200000000000003</v>
       </c>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="171" t="s">
+      <c r="F3" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="169">
+      <c r="G3" s="168">
         <v>2</v>
       </c>
-      <c r="H3" s="165" t="s">
+      <c r="H3" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="258"/>
+      <c r="I3" s="257"/>
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="171">
+      <c r="C4" s="170">
         <v>-103.7</v>
       </c>
-      <c r="D4" s="171">
+      <c r="D4" s="170">
         <v>-111.3</v>
       </c>
-      <c r="E4" s="171" t="s">
+      <c r="E4" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="171" t="s">
+      <c r="F4" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="169">
+      <c r="G4" s="168">
         <v>2</v>
       </c>
-      <c r="H4" s="165" t="s">
+      <c r="H4" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="258"/>
+      <c r="I4" s="257"/>
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="171" t="s">
+      <c r="B5" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="171">
+      <c r="C5" s="170">
         <v>16.399999999999999</v>
       </c>
-      <c r="D5" s="171" t="s">
+      <c r="D5" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="171" t="s">
+      <c r="E5" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="171" t="s">
+      <c r="F5" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="169">
+      <c r="G5" s="168">
         <v>2</v>
       </c>
-      <c r="H5" s="165" t="s">
+      <c r="H5" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="258"/>
+      <c r="I5" s="257"/>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="171">
+      <c r="B6" s="170">
         <f>-386</f>
         <v>-386</v>
       </c>
-      <c r="C6" s="171">
+      <c r="C6" s="170">
         <v>-623.16</v>
       </c>
-      <c r="D6" s="171">
+      <c r="D6" s="170">
         <v>-586.85</v>
       </c>
-      <c r="E6" s="171">
+      <c r="E6" s="170">
         <v>-527.79999999999995</v>
       </c>
-      <c r="F6" s="171" t="s">
+      <c r="F6" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="169">
+      <c r="G6" s="168">
         <v>3</v>
       </c>
-      <c r="H6" s="165" t="s">
+      <c r="H6" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="258"/>
+      <c r="I6" s="257"/>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="174" t="s">
         <v>92</v>
       </c>
-      <c r="C7" s="175">
+      <c r="C7" s="174">
         <v>-755.9</v>
       </c>
-      <c r="D7" s="175">
+      <c r="D7" s="174">
         <f>-180.69*4.184</f>
         <v>-756.00696000000005</v>
       </c>
-      <c r="E7" s="175">
+      <c r="E7" s="174">
         <f>-177.97*4.184</f>
         <v>-744.62648000000002</v>
       </c>
-      <c r="F7" s="175" t="s">
+      <c r="F7" s="174" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="170">
+      <c r="G7" s="169">
         <v>4</v>
       </c>
       <c r="H7" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="258"/>
+      <c r="I7" s="257"/>
     </row>
     <row r="8" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="150" t="s">
+      <c r="A8" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="177" t="s">
+      <c r="B8" s="176" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="177">
-        <v>0</v>
-      </c>
-      <c r="D8" s="177" t="s">
+      <c r="C8" s="176">
+        <v>0</v>
+      </c>
+      <c r="D8" s="176" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="177" t="s">
+      <c r="E8" s="176" t="s">
         <v>92</v>
       </c>
-      <c r="F8" s="178" t="s">
+      <c r="F8" s="177" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="197">
+      <c r="G8" s="196">
         <v>2</v>
       </c>
       <c r="H8" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="258"/>
+      <c r="I8" s="257"/>
     </row>
     <row r="9" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="179" t="s">
+      <c r="B9" s="178" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="177">
-        <v>0</v>
-      </c>
-      <c r="D9" s="177" t="s">
+      <c r="C9" s="176">
+        <v>0</v>
+      </c>
+      <c r="D9" s="176" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="177" t="s">
+      <c r="E9" s="176" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="178" t="s">
+      <c r="F9" s="177" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="197">
+      <c r="G9" s="196">
         <v>2</v>
       </c>
       <c r="H9" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="258"/>
+      <c r="I9" s="257"/>
     </row>
     <row r="10" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="159" t="s">
+      <c r="A10" s="158" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="176" t="s">
+      <c r="B10" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="176">
+      <c r="C10" s="175">
         <v>-237.18</v>
       </c>
-      <c r="D10" s="176">
+      <c r="D10" s="175">
         <v>-157.30000000000001</v>
       </c>
-      <c r="E10" s="176" t="s">
+      <c r="E10" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="176" t="s">
+      <c r="F10" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="196">
+      <c r="G10" s="195">
         <v>2</v>
       </c>
       <c r="H10" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="258"/>
+      <c r="I10" s="257"/>
     </row>
     <row r="11" spans="1:9" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="160" t="s">
+      <c r="A11" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="171" t="s">
+      <c r="B11" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="C11" s="171">
-        <v>0</v>
-      </c>
-      <c r="D11" s="171" t="s">
+      <c r="C11" s="170">
+        <v>0</v>
+      </c>
+      <c r="D11" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="171" t="s">
+      <c r="E11" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="F11" s="171" t="s">
+      <c r="F11" s="170" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="170">
+      <c r="G11" s="169">
         <v>2</v>
       </c>
       <c r="H11" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="258"/>
+      <c r="I11" s="257"/>
     </row>
     <row r="12" spans="1:9" s="71" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="161" t="s">
+      <c r="A12" s="160" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="166" t="s">
+      <c r="B12" s="165" t="s">
         <v>239</v>
       </c>
-      <c r="C12" s="166" t="s">
+      <c r="C12" s="165" t="s">
         <v>240</v>
       </c>
-      <c r="D12" s="167" t="s">
+      <c r="D12" s="166" t="s">
         <v>241</v>
       </c>
-      <c r="E12" s="166" t="s">
+      <c r="E12" s="165" t="s">
         <v>242</v>
       </c>
       <c r="H12" s="72"/>
@@ -5157,24 +5241,24 @@
       <c r="A13" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="172">
+      <c r="B13" s="171">
         <f>IF(COUNT(B2,C2)=2, EXP(($C$10+B2-C2)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C13" s="156">
+      <c r="C13" s="155">
         <f>IF(COUNT(C2,D2)=2, EXP((D2-C2)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>3.9083870641861443E-10</v>
       </c>
-      <c r="D13" s="172">
+      <c r="D13" s="171">
         <f>IF(COUNT(D2,E2)=2, EXP((E2-D2)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="172">
+      <c r="E13" s="171">
         <f>IF(COUNT(E2,F2)=2, EXP((F2-E2)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="257" t="s">
+      <c r="I13" s="256" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5182,170 +5266,170 @@
       <c r="A14" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="172">
+      <c r="B14" s="171">
         <f>IF(COUNT(B3,C3)=2, EXP(($C$10+B3-C3)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="156">
+      <c r="C14" s="155">
         <f>IF(COUNT(C3,D3)=2, EXP((D3-C3)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>5.2656707191475868E-4</v>
       </c>
-      <c r="D14" s="172">
+      <c r="D14" s="171">
         <f>IF(COUNT(D3,E3)=2, EXP((E3-D3)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="172">
+      <c r="E14" s="171">
         <f>IF(COUNT(E3,F3)=2, EXP((F3-E3)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="257"/>
+      <c r="I14" s="256"/>
     </row>
     <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="172">
+      <c r="B15" s="171">
         <f>IF(COUNT(B4,C4)=2, EXP(($C$10+B4-C4)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="156">
+      <c r="C15" s="155">
         <f>IF(COUNT(C4,D4)=2, EXP((D4-C4)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>22.603837077490315</v>
       </c>
-      <c r="D15" s="172">
+      <c r="D15" s="171">
         <f>IF(COUNT(D4,E4)=2, EXP((E4-D4)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="172">
+      <c r="E15" s="171">
         <f>IF(COUNT(E4,F4)=2, EXP((F4-E4)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="257"/>
+      <c r="I15" s="256"/>
     </row>
     <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="172">
+      <c r="B16" s="171">
         <f>IF(COUNT(B5,C5)=2, EXP(($C$10+B5-C5)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C16" s="172">
+      <c r="C16" s="171">
         <f>IF(COUNT(C5,D5)=2, EXP((D5-C5)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="172">
+      <c r="D16" s="171">
         <f>IF(COUNT(D5,E5)=2, EXP((E5-D5)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="172">
+      <c r="E16" s="171">
         <f>IF(COUNT(E5,F5)=2, EXP((F5-E5)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="257"/>
+      <c r="I16" s="256"/>
     </row>
     <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="173">
+      <c r="B17" s="172">
         <f>1/0.0017</f>
         <v>588.23529411764707</v>
       </c>
-      <c r="C17" s="156">
+      <c r="C17" s="155">
         <f>IF(COUNT(C6,D6)=2, EXP((D6-C6)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>3.3901312221699524E-7</v>
       </c>
-      <c r="D17" s="156">
+      <c r="D17" s="155">
         <f>IF(COUNT(D6,E6)=2, EXP((E6-D6)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>3.008575507210982E-11</v>
       </c>
-      <c r="E17" s="172">
+      <c r="E17" s="171">
         <f>IF(COUNT(E6,F6)=2, EXP((F6-E6)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="257"/>
+      <c r="I17" s="256"/>
     </row>
     <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="181">
+      <c r="B18" s="180">
         <f>IF(COUNT(B7,C7)=2, EXP(($C$10+B7-C7)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="194">
+      <c r="C18" s="193">
         <v>100</v>
       </c>
-      <c r="D18" s="195">
+      <c r="D18" s="194">
         <f>10^(-1.92)</f>
         <v>1.2022644346174125E-2</v>
       </c>
-      <c r="E18" s="182">
+      <c r="E18" s="181">
         <f>IF(COUNT(E7,F7)=2, EXP((F7-E7)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F18" s="71"/>
       <c r="H18" s="71"/>
-      <c r="I18" s="257"/>
+      <c r="I18" s="256"/>
     </row>
     <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="150" t="s">
+      <c r="A19" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="192">
+      <c r="B19" s="191">
         <f>IF(COUNT(B8,C8)=2, EXP(($C$10+B8-C8)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C19" s="193">
+      <c r="C19" s="192">
         <f>IF(COUNT(C8,D8)=2, EXP((D8-C8)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="193">
+      <c r="D19" s="192">
         <f>IF(COUNT(D8,E8)=2, EXP((E8-D8)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="193">
+      <c r="E19" s="192">
         <f>IF(COUNT(E8,F8)=2, EXP((F8-E8)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F19" s="71"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="257"/>
+      <c r="I19" s="256"/>
     </row>
     <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="150" t="s">
+      <c r="A20" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="183">
+      <c r="B20" s="182">
         <f>IF(COUNT(B9,C9)=2, EXP(($C$10+B9-C9)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C20" s="184">
+      <c r="C20" s="183">
         <f>IF(COUNT(C9,D9)=2, EXP((D9-C9)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="184">
+      <c r="D20" s="183">
         <f>IF(COUNT(D9,E9)=2, EXP((E9-D9)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="184">
+      <c r="E20" s="183">
         <f>IF(COUNT(E9,F9)=2, EXP((F9-E9)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="257"/>
+      <c r="I20" s="256"/>
     </row>
     <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="159" t="s">
+      <c r="A21" s="158" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="180">
+      <c r="B21" s="179">
         <f>IF(COUNT(B10,C10)=2, EXP(($C$10+B10-C10)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
@@ -5353,71 +5437,71 @@
         <f>IF(COUNT(C10,D10)=2, EXP((D10-C10)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>5.845648305092005E-15</v>
       </c>
-      <c r="D21" s="180">
+      <c r="D21" s="179">
         <f>IF(COUNT(D10,E10)=2, EXP((E10-D10)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="180">
+      <c r="E21" s="179">
         <f>IF(COUNT(E10,F10)=2, EXP((F10-E10)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="257"/>
+      <c r="I21" s="256"/>
     </row>
     <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="160" t="s">
+      <c r="A22" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="172">
+      <c r="B22" s="171">
         <f>IF(COUNT(B11,C11)=2, EXP(($C$10+B11-C11)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="C22" s="172">
+      <c r="C22" s="171">
         <f>IF(COUNT(C11,D11)=2, EXP((D11-C11)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="172">
+      <c r="D22" s="171">
         <f>IF(COUNT(D11,E11)=2, EXP((E11-D11)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="172">
+      <c r="E22" s="171">
         <f>IF(COUNT(E11,F11)=2, EXP((F11-E11)/-(Parameters!$B$9*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="257"/>
+      <c r="I22" s="256"/>
     </row>
     <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="259" t="s">
+      <c r="A23" s="258" t="s">
         <v>238</v>
       </c>
-      <c r="B23" s="260"/>
-      <c r="C23" s="260"/>
-      <c r="D23" s="260"/>
-      <c r="E23" s="260"/>
-      <c r="F23" s="261"/>
+      <c r="B23" s="259"/>
+      <c r="C23" s="259"/>
+      <c r="D23" s="259"/>
+      <c r="E23" s="259"/>
+      <c r="F23" s="260"/>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="174" t="s">
+      <c r="B24" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="174">
+      <c r="C24" s="173">
         <v>1</v>
       </c>
-      <c r="D24" s="174">
-        <v>0</v>
-      </c>
-      <c r="E24" s="174" t="s">
+      <c r="D24" s="173">
+        <v>0</v>
+      </c>
+      <c r="E24" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="F24" s="174" t="s">
+      <c r="F24" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="257" t="s">
+      <c r="I24" s="256" t="s">
         <v>253</v>
       </c>
     </row>
@@ -5425,190 +5509,190 @@
       <c r="A25" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="174" t="s">
+      <c r="B25" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="174">
-        <v>0</v>
-      </c>
-      <c r="D25" s="174">
+      <c r="C25" s="173">
+        <v>0</v>
+      </c>
+      <c r="D25" s="173">
         <v>-1</v>
       </c>
-      <c r="E25" s="174" t="s">
+      <c r="E25" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="F25" s="174" t="s">
+      <c r="F25" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="257"/>
+      <c r="I25" s="256"/>
     </row>
     <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="174" t="s">
+      <c r="B26" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="174">
-        <v>0</v>
-      </c>
-      <c r="D26" s="174">
+      <c r="C26" s="173">
+        <v>0</v>
+      </c>
+      <c r="D26" s="173">
         <v>-1</v>
       </c>
-      <c r="E26" s="174" t="s">
+      <c r="E26" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="174" t="s">
+      <c r="F26" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="257"/>
+      <c r="I26" s="256"/>
     </row>
     <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="174" t="s">
+      <c r="B27" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="174">
-        <v>0</v>
-      </c>
-      <c r="D27" s="174" t="s">
+      <c r="C27" s="173">
+        <v>0</v>
+      </c>
+      <c r="D27" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="174" t="s">
+      <c r="E27" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="174" t="s">
+      <c r="F27" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I27" s="257"/>
+      <c r="I27" s="256"/>
     </row>
     <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="174">
-        <v>0</v>
-      </c>
-      <c r="C28" s="174">
-        <v>0</v>
-      </c>
-      <c r="D28" s="174">
+      <c r="B28" s="173">
+        <v>0</v>
+      </c>
+      <c r="C28" s="173">
+        <v>0</v>
+      </c>
+      <c r="D28" s="173">
         <v>-1</v>
       </c>
-      <c r="E28" s="174">
+      <c r="E28" s="173">
         <v>-2</v>
       </c>
-      <c r="F28" s="174" t="s">
+      <c r="F28" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="257"/>
+      <c r="I28" s="256"/>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="186" t="s">
+      <c r="B29" s="185" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="187">
-        <v>0</v>
-      </c>
-      <c r="D29" s="187">
+      <c r="C29" s="186">
+        <v>0</v>
+      </c>
+      <c r="D29" s="186">
         <v>-1</v>
       </c>
-      <c r="E29" s="187">
+      <c r="E29" s="186">
         <v>-2</v>
       </c>
-      <c r="F29" s="187" t="s">
+      <c r="F29" s="186" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="257"/>
+      <c r="I29" s="256"/>
     </row>
     <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="150" t="s">
+      <c r="A30" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="190" t="s">
+      <c r="B30" s="189" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="191">
+      <c r="C30" s="190">
         <v>1</v>
       </c>
-      <c r="D30" s="191" t="s">
+      <c r="D30" s="190" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="191" t="s">
+      <c r="E30" s="190" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="191" t="s">
+      <c r="F30" s="190" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="257"/>
+      <c r="I30" s="256"/>
     </row>
     <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="150" t="s">
+      <c r="A31" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="188" t="s">
+      <c r="B31" s="187" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="189">
-        <v>0</v>
-      </c>
-      <c r="D31" s="189" t="s">
+      <c r="C31" s="188">
+        <v>0</v>
+      </c>
+      <c r="D31" s="188" t="s">
         <v>93</v>
       </c>
-      <c r="E31" s="189" t="s">
+      <c r="E31" s="188" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="189" t="s">
+      <c r="F31" s="188" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="257"/>
+      <c r="I31" s="256"/>
     </row>
     <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="159" t="s">
+      <c r="A32" s="158" t="s">
         <v>86</v>
       </c>
-      <c r="B32" s="185" t="s">
+      <c r="B32" s="184" t="s">
         <v>93</v>
       </c>
-      <c r="C32" s="185">
-        <v>0</v>
-      </c>
-      <c r="D32" s="185">
+      <c r="C32" s="184">
+        <v>0</v>
+      </c>
+      <c r="D32" s="184">
         <v>-1</v>
       </c>
-      <c r="E32" s="185" t="s">
+      <c r="E32" s="184" t="s">
         <v>93</v>
       </c>
-      <c r="F32" s="185" t="s">
+      <c r="F32" s="184" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="257"/>
+      <c r="I32" s="256"/>
     </row>
     <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="160" t="s">
+      <c r="A33" s="159" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="174" t="s">
+      <c r="B33" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="174">
+      <c r="C33" s="173">
         <v>1</v>
       </c>
-      <c r="D33" s="174" t="s">
+      <c r="D33" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="E33" s="174" t="s">
+      <c r="E33" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="174" t="s">
+      <c r="F33" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="257"/>
+      <c r="I33" s="256"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5618,15 +5702,15 @@
     <mergeCell ref="I24:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:F11 B24:F33 B13:E17 B19:E22 B18 D18:E18">
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="59" priority="54" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="58" priority="55" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:E17 B19:E22 B18 D18:E18">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5641,7 +5725,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5656,19 +5740,19 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="155" t="s">
+      <c r="C1" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="155" t="s">
+      <c r="D1" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="155" t="s">
+      <c r="E1" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="249" t="s">
+      <c r="F1" s="248" t="s">
         <v>249</v>
       </c>
     </row>
@@ -5676,95 +5760,95 @@
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="156">
+      <c r="B2" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C2" s="156">
-        <v>0</v>
-      </c>
-      <c r="D2" s="156">
-        <v>0</v>
-      </c>
-      <c r="E2" s="156">
+      <c r="C2" s="155">
+        <v>0</v>
+      </c>
+      <c r="D2" s="155">
+        <v>0</v>
+      </c>
+      <c r="E2" s="155">
         <f>(0.1/32)/1000</f>
         <v>3.1250000000000001E-6</v>
       </c>
-      <c r="F2" s="249"/>
+      <c r="F2" s="248"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B3" s="156">
-        <v>0</v>
-      </c>
-      <c r="C3" s="156">
+        <v>275</v>
+      </c>
+      <c r="B3" s="155">
+        <v>0</v>
+      </c>
+      <c r="C3" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D3" s="156">
-        <v>0</v>
-      </c>
-      <c r="E3" s="156">
+      <c r="D3" s="155">
+        <v>0</v>
+      </c>
+      <c r="E3" s="155">
         <f t="shared" ref="E3:E6" si="0">(0.1/32)/1000</f>
         <v>3.1250000000000001E-6</v>
       </c>
-      <c r="F3" s="249"/>
+      <c r="F3" s="248"/>
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="156">
+      <c r="B4" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C4" s="156">
+      <c r="C4" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D4" s="156">
-        <v>0</v>
-      </c>
-      <c r="E4" s="156">
-        <v>0</v>
-      </c>
-      <c r="F4" s="249"/>
+      <c r="D4" s="155">
+        <v>0</v>
+      </c>
+      <c r="E4" s="155">
+        <v>0</v>
+      </c>
+      <c r="F4" s="248"/>
     </row>
     <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="156">
+      <c r="B5" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C5" s="156">
-        <v>0</v>
-      </c>
-      <c r="D5" s="156">
-        <v>0</v>
-      </c>
-      <c r="E5" s="156">
+      <c r="C5" s="155">
+        <v>0</v>
+      </c>
+      <c r="D5" s="155">
+        <v>0</v>
+      </c>
+      <c r="E5" s="155">
         <f t="shared" si="0"/>
         <v>3.1250000000000001E-6</v>
       </c>
-      <c r="F5" s="249"/>
+      <c r="F5" s="248"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="89" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="156">
+      <c r="B6" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C6" s="156">
-        <v>0</v>
-      </c>
-      <c r="D6" s="156">
+      <c r="C6" s="155">
+        <v>0</v>
+      </c>
+      <c r="D6" s="155">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E6" s="156">
+      <c r="E6" s="155">
         <f t="shared" si="0"/>
         <v>3.1250000000000001E-6</v>
       </c>
-      <c r="F6" s="249"/>
+      <c r="F6" s="248"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5772,7 +5856,7 @@
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
   <conditionalFormatting sqref="B2:E6">
-    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5798,16 +5882,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
-      <c r="B1" s="155" t="s">
+      <c r="B1" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="155" t="s">
+      <c r="C1" s="154" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="155" t="s">
+      <c r="D1" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="249" t="s">
+      <c r="E1" s="248" t="s">
         <v>248</v>
       </c>
     </row>
@@ -5815,84 +5899,84 @@
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="156">
-        <v>0</v>
-      </c>
-      <c r="C2" s="156">
-        <v>0</v>
-      </c>
-      <c r="D2" s="156">
-        <v>0</v>
-      </c>
-      <c r="E2" s="249"/>
+      <c r="B2" s="155">
+        <v>0</v>
+      </c>
+      <c r="C2" s="155">
+        <v>0</v>
+      </c>
+      <c r="D2" s="155">
+        <v>0</v>
+      </c>
+      <c r="E2" s="248"/>
     </row>
     <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B3" s="156">
-        <v>0</v>
-      </c>
-      <c r="C3" s="156">
-        <v>0</v>
-      </c>
-      <c r="D3" s="156">
-        <v>0</v>
-      </c>
-      <c r="E3" s="249"/>
+        <v>275</v>
+      </c>
+      <c r="B3" s="155">
+        <v>0</v>
+      </c>
+      <c r="C3" s="155">
+        <v>0</v>
+      </c>
+      <c r="D3" s="155">
+        <v>0</v>
+      </c>
+      <c r="E3" s="248"/>
     </row>
     <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="156">
-        <v>0</v>
-      </c>
-      <c r="C4" s="156">
-        <v>0</v>
-      </c>
-      <c r="D4" s="156">
+      <c r="B4" s="155">
+        <v>0</v>
+      </c>
+      <c r="C4" s="155">
+        <v>0</v>
+      </c>
+      <c r="D4" s="155">
         <f>0.1*(1/32)*(1/1000)</f>
         <v>3.1250000000000001E-6</v>
       </c>
-      <c r="E4" s="249"/>
+      <c r="E4" s="248"/>
     </row>
     <row r="5" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="156">
-        <v>0</v>
-      </c>
-      <c r="C5" s="156">
-        <v>0</v>
-      </c>
-      <c r="D5" s="156">
-        <v>0</v>
-      </c>
-      <c r="E5" s="249"/>
+      <c r="B5" s="155">
+        <v>0</v>
+      </c>
+      <c r="C5" s="155">
+        <v>0</v>
+      </c>
+      <c r="D5" s="155">
+        <v>0</v>
+      </c>
+      <c r="E5" s="248"/>
     </row>
     <row r="6" spans="1:5" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="89" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="156">
-        <v>0</v>
-      </c>
-      <c r="C6" s="156">
-        <v>0</v>
-      </c>
-      <c r="D6" s="156">
-        <v>0</v>
-      </c>
-      <c r="E6" s="249"/>
+      <c r="B6" s="155">
+        <v>0</v>
+      </c>
+      <c r="C6" s="155">
+        <v>0</v>
+      </c>
+      <c r="D6" s="155">
+        <v>0</v>
+      </c>
+      <c r="E6" s="248"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:D6">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5919,16 +6003,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="155" t="s">
-        <v>279</v>
-      </c>
-      <c r="C1" s="155" t="s">
+      <c r="B1" s="154" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="155" t="s">
+      <c r="D1" s="154" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="155" t="s">
+      <c r="E1" s="154" t="s">
         <v>247</v>
       </c>
     </row>
@@ -5936,94 +6020,94 @@
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="156">
+      <c r="B2" s="155">
         <f>0.0415</f>
         <v>4.1500000000000002E-2</v>
       </c>
-      <c r="C2" s="157" t="s">
+      <c r="C2" s="156" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="158">
+      <c r="D2" s="157">
         <v>1E-3</v>
       </c>
-      <c r="E2" s="158">
+      <c r="E2" s="157">
         <v>0.01</v>
       </c>
-      <c r="F2" s="258" t="s">
-        <v>276</v>
+      <c r="F2" s="257" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
-        <v>278</v>
-      </c>
-      <c r="B3" s="156">
+        <v>275</v>
+      </c>
+      <c r="B3" s="155">
         <v>2.07E-2</v>
       </c>
-      <c r="C3" s="157" t="s">
+      <c r="C3" s="156" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="158">
+      <c r="D3" s="157">
         <v>1E-3</v>
       </c>
-      <c r="E3" s="158">
+      <c r="E3" s="157">
         <v>0.01</v>
       </c>
-      <c r="F3" s="258"/>
+      <c r="F3" s="257"/>
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="156">
+      <c r="B4" s="155">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="156" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="158">
+      <c r="D4" s="157">
         <v>1E-3</v>
       </c>
-      <c r="E4" s="158">
+      <c r="E4" s="157">
         <v>0.01</v>
       </c>
-      <c r="F4" s="258"/>
+      <c r="F4" s="257"/>
     </row>
     <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="156">
+      <c r="B5" s="155">
         <v>6.2199999999999998E-2</v>
       </c>
-      <c r="C5" s="156" t="s">
+      <c r="C5" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="158">
+      <c r="D5" s="157">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="158">
+      <c r="E5" s="157">
         <v>0.01</v>
       </c>
-      <c r="F5" s="258"/>
+      <c r="F5" s="257"/>
     </row>
     <row r="6" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="89" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="156">
+      <c r="B6" s="155">
         <v>1.7399999999999999E-2</v>
       </c>
-      <c r="C6" s="156" t="s">
+      <c r="C6" s="155" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="158">
+      <c r="D6" s="157">
         <v>1E-3</v>
       </c>
-      <c r="E6" s="158">
+      <c r="E6" s="157">
         <v>0.01</v>
       </c>
-      <c r="F6" s="258"/>
+      <c r="F6" s="257"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6042,7 +6126,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6059,77 +6143,77 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
-      <c r="B1" s="264" t="s">
+      <c r="B1" s="263" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="262"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="264" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="262"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="262" t="s">
+      <c r="C1" s="261"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="263" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="261"/>
+      <c r="G1" s="262"/>
+      <c r="H1" s="261" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="262"/>
-      <c r="J1" s="263"/>
-      <c r="K1" s="262" t="s">
+      <c r="I1" s="261"/>
+      <c r="J1" s="262"/>
+      <c r="K1" s="261" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="262"/>
-      <c r="M1" s="263"/>
-      <c r="N1" s="262" t="s">
+      <c r="L1" s="261"/>
+      <c r="M1" s="262"/>
+      <c r="N1" s="261" t="s">
         <v>121</v>
       </c>
-      <c r="O1" s="262"/>
-      <c r="P1" s="263"/>
+      <c r="O1" s="261"/>
+      <c r="P1" s="262"/>
     </row>
     <row r="2" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="200" t="s">
+      <c r="C2" s="199" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="201" t="s">
+      <c r="D2" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="199" t="s">
+      <c r="E2" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="200" t="s">
+      <c r="F2" s="199" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="201" t="s">
+      <c r="G2" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="200" t="s">
+      <c r="H2" s="199" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="200" t="s">
+      <c r="I2" s="199" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="201" t="s">
+      <c r="J2" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="200" t="s">
+      <c r="K2" s="199" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="200" t="s">
+      <c r="L2" s="199" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="201" t="s">
+      <c r="M2" s="200" t="s">
         <v>79</v>
       </c>
-      <c r="N2" s="200" t="s">
+      <c r="N2" s="199" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="200" t="s">
+      <c r="O2" s="199" t="s">
         <v>78</v>
       </c>
-      <c r="P2" s="201" t="s">
+      <c r="P2" s="200" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6137,49 +6221,49 @@
       <c r="A3" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="205">
+      <c r="B3" s="204">
         <v>-1</v>
       </c>
       <c r="C3" s="105">
         <v>0</v>
       </c>
-      <c r="D3" s="206">
-        <v>0</v>
-      </c>
-      <c r="E3" s="205">
+      <c r="D3" s="205">
+        <v>0</v>
+      </c>
+      <c r="E3" s="204">
         <v>0</v>
       </c>
       <c r="F3" s="105">
         <v>0</v>
       </c>
-      <c r="G3" s="206">
-        <v>0</v>
-      </c>
-      <c r="H3" s="205">
+      <c r="G3" s="205">
+        <v>0</v>
+      </c>
+      <c r="H3" s="204">
         <v>-1</v>
       </c>
       <c r="I3" s="105">
         <v>0</v>
       </c>
-      <c r="J3" s="206">
-        <v>0</v>
-      </c>
-      <c r="K3" s="205">
+      <c r="J3" s="205">
+        <v>0</v>
+      </c>
+      <c r="K3" s="204">
         <v>-1</v>
       </c>
       <c r="L3" s="105">
         <v>0</v>
       </c>
-      <c r="M3" s="206">
-        <v>0</v>
-      </c>
-      <c r="N3" s="205">
+      <c r="M3" s="205">
+        <v>0</v>
+      </c>
+      <c r="N3" s="204">
         <v>-1</v>
       </c>
       <c r="O3" s="105">
         <v>0</v>
       </c>
-      <c r="P3" s="206">
+      <c r="P3" s="205">
         <v>0</v>
       </c>
     </row>
@@ -6187,49 +6271,49 @@
       <c r="A4" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="207">
+      <c r="B4" s="206">
         <v>1</v>
       </c>
-      <c r="C4" s="208">
-        <v>0</v>
-      </c>
-      <c r="D4" s="209">
-        <v>0</v>
-      </c>
-      <c r="E4" s="207">
+      <c r="C4" s="207">
+        <v>0</v>
+      </c>
+      <c r="D4" s="208">
+        <v>0</v>
+      </c>
+      <c r="E4" s="206">
         <v>-1</v>
       </c>
-      <c r="F4" s="208">
-        <v>0</v>
-      </c>
-      <c r="G4" s="209">
-        <v>0</v>
-      </c>
-      <c r="H4" s="207">
+      <c r="F4" s="207">
+        <v>0</v>
+      </c>
+      <c r="G4" s="208">
+        <v>0</v>
+      </c>
+      <c r="H4" s="206">
         <v>-1</v>
       </c>
-      <c r="I4" s="208">
-        <v>0</v>
-      </c>
-      <c r="J4" s="209">
-        <v>0</v>
-      </c>
-      <c r="K4" s="207">
-        <v>0</v>
-      </c>
-      <c r="L4" s="208">
-        <v>0</v>
-      </c>
-      <c r="M4" s="209">
-        <v>0</v>
-      </c>
-      <c r="N4" s="207">
+      <c r="I4" s="207">
+        <v>0</v>
+      </c>
+      <c r="J4" s="208">
+        <v>0</v>
+      </c>
+      <c r="K4" s="206">
+        <v>0</v>
+      </c>
+      <c r="L4" s="207">
+        <v>0</v>
+      </c>
+      <c r="M4" s="208">
+        <v>0</v>
+      </c>
+      <c r="N4" s="206">
         <v>2</v>
       </c>
-      <c r="O4" s="208">
-        <v>0</v>
-      </c>
-      <c r="P4" s="209">
+      <c r="O4" s="207">
+        <v>0</v>
+      </c>
+      <c r="P4" s="208">
         <v>0</v>
       </c>
     </row>
@@ -6237,49 +6321,49 @@
       <c r="A5" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="207">
-        <v>0</v>
-      </c>
-      <c r="C5" s="208">
-        <v>0</v>
-      </c>
-      <c r="D5" s="209">
-        <v>0</v>
-      </c>
-      <c r="E5" s="207">
+      <c r="B5" s="206">
+        <v>0</v>
+      </c>
+      <c r="C5" s="207">
+        <v>0</v>
+      </c>
+      <c r="D5" s="208">
+        <v>0</v>
+      </c>
+      <c r="E5" s="206">
         <v>1</v>
       </c>
-      <c r="F5" s="208">
-        <v>0</v>
-      </c>
-      <c r="G5" s="209">
-        <v>0</v>
-      </c>
-      <c r="H5" s="207">
-        <v>0</v>
-      </c>
-      <c r="I5" s="208">
-        <v>0</v>
-      </c>
-      <c r="J5" s="209">
-        <v>0</v>
-      </c>
-      <c r="K5" s="207">
+      <c r="F5" s="207">
+        <v>0</v>
+      </c>
+      <c r="G5" s="208">
+        <v>0</v>
+      </c>
+      <c r="H5" s="206">
+        <v>0</v>
+      </c>
+      <c r="I5" s="207">
+        <v>0</v>
+      </c>
+      <c r="J5" s="208">
+        <v>0</v>
+      </c>
+      <c r="K5" s="206">
         <v>1</v>
       </c>
-      <c r="L5" s="208">
-        <v>0</v>
-      </c>
-      <c r="M5" s="209">
-        <v>0</v>
-      </c>
-      <c r="N5" s="207">
+      <c r="L5" s="207">
+        <v>0</v>
+      </c>
+      <c r="M5" s="208">
+        <v>0</v>
+      </c>
+      <c r="N5" s="206">
         <v>-1</v>
       </c>
-      <c r="O5" s="208">
-        <v>0</v>
-      </c>
-      <c r="P5" s="209">
+      <c r="O5" s="207">
+        <v>0</v>
+      </c>
+      <c r="P5" s="208">
         <v>0</v>
       </c>
     </row>
@@ -6287,49 +6371,49 @@
       <c r="A6" s="77" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="207">
+      <c r="B6" s="206">
         <v>-1.5</v>
       </c>
-      <c r="C6" s="208">
-        <v>0</v>
-      </c>
-      <c r="D6" s="209">
-        <v>0</v>
-      </c>
-      <c r="E6" s="207">
+      <c r="C6" s="207">
+        <v>0</v>
+      </c>
+      <c r="D6" s="208">
+        <v>0</v>
+      </c>
+      <c r="E6" s="206">
         <v>-0.5</v>
       </c>
-      <c r="F6" s="208">
-        <v>0</v>
-      </c>
-      <c r="G6" s="209">
-        <v>0</v>
-      </c>
-      <c r="H6" s="207">
-        <v>0</v>
-      </c>
-      <c r="I6" s="208">
-        <v>0</v>
-      </c>
-      <c r="J6" s="209">
-        <v>0</v>
-      </c>
-      <c r="K6" s="207">
+      <c r="F6" s="207">
+        <v>0</v>
+      </c>
+      <c r="G6" s="208">
+        <v>0</v>
+      </c>
+      <c r="H6" s="206">
+        <v>0</v>
+      </c>
+      <c r="I6" s="207">
+        <v>0</v>
+      </c>
+      <c r="J6" s="208">
+        <v>0</v>
+      </c>
+      <c r="K6" s="206">
         <v>-2</v>
       </c>
-      <c r="L6" s="208">
-        <v>0</v>
-      </c>
-      <c r="M6" s="209">
-        <v>0</v>
-      </c>
-      <c r="N6" s="207">
+      <c r="L6" s="207">
+        <v>0</v>
+      </c>
+      <c r="M6" s="208">
+        <v>0</v>
+      </c>
+      <c r="N6" s="206">
         <v>-1</v>
       </c>
-      <c r="O6" s="208">
-        <v>0</v>
-      </c>
-      <c r="P6" s="209">
+      <c r="O6" s="207">
+        <v>0</v>
+      </c>
+      <c r="P6" s="208">
         <v>0</v>
       </c>
     </row>
@@ -6337,49 +6421,49 @@
       <c r="A7" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="207">
-        <v>0</v>
-      </c>
-      <c r="C7" s="208">
+      <c r="B7" s="206">
+        <v>0</v>
+      </c>
+      <c r="C7" s="207">
         <v>-1</v>
       </c>
-      <c r="D7" s="209">
+      <c r="D7" s="208">
         <v>1</v>
       </c>
-      <c r="E7" s="207">
-        <v>0</v>
-      </c>
-      <c r="F7" s="208">
+      <c r="E7" s="206">
+        <v>0</v>
+      </c>
+      <c r="F7" s="207">
         <v>-1</v>
       </c>
-      <c r="G7" s="209">
+      <c r="G7" s="208">
         <v>1</v>
       </c>
-      <c r="H7" s="207">
-        <v>0</v>
-      </c>
-      <c r="I7" s="208">
+      <c r="H7" s="206">
+        <v>0</v>
+      </c>
+      <c r="I7" s="207">
         <v>-1</v>
       </c>
-      <c r="J7" s="209">
+      <c r="J7" s="208">
         <v>1</v>
       </c>
-      <c r="K7" s="207">
-        <v>0</v>
-      </c>
-      <c r="L7" s="208">
+      <c r="K7" s="206">
+        <v>0</v>
+      </c>
+      <c r="L7" s="207">
         <v>-1</v>
       </c>
-      <c r="M7" s="209">
+      <c r="M7" s="208">
         <v>1</v>
       </c>
-      <c r="N7" s="207">
-        <v>0</v>
-      </c>
-      <c r="O7" s="208">
+      <c r="N7" s="206">
+        <v>0</v>
+      </c>
+      <c r="O7" s="207">
         <v>-1</v>
       </c>
-      <c r="P7" s="209">
+      <c r="P7" s="208">
         <v>1</v>
       </c>
     </row>
@@ -6387,249 +6471,249 @@
       <c r="A8" s="77" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="210">
-        <v>0</v>
-      </c>
-      <c r="C8" s="202">
-        <v>0</v>
-      </c>
-      <c r="D8" s="211">
-        <v>0</v>
-      </c>
-      <c r="E8" s="210">
-        <v>0</v>
-      </c>
-      <c r="F8" s="202">
-        <v>0</v>
-      </c>
-      <c r="G8" s="211">
-        <v>0</v>
-      </c>
-      <c r="H8" s="210">
-        <v>0</v>
-      </c>
-      <c r="I8" s="202">
-        <v>0</v>
-      </c>
-      <c r="J8" s="211">
-        <v>0</v>
-      </c>
-      <c r="K8" s="210">
-        <v>0</v>
-      </c>
-      <c r="L8" s="202">
-        <v>0</v>
-      </c>
-      <c r="M8" s="211">
-        <v>0</v>
-      </c>
-      <c r="N8" s="210">
-        <v>0</v>
-      </c>
-      <c r="O8" s="202">
-        <v>0</v>
-      </c>
-      <c r="P8" s="211">
+      <c r="B8" s="209">
+        <v>0</v>
+      </c>
+      <c r="C8" s="201">
+        <v>0</v>
+      </c>
+      <c r="D8" s="210">
+        <v>0</v>
+      </c>
+      <c r="E8" s="209">
+        <v>0</v>
+      </c>
+      <c r="F8" s="201">
+        <v>0</v>
+      </c>
+      <c r="G8" s="210">
+        <v>0</v>
+      </c>
+      <c r="H8" s="209">
+        <v>0</v>
+      </c>
+      <c r="I8" s="201">
+        <v>0</v>
+      </c>
+      <c r="J8" s="210">
+        <v>0</v>
+      </c>
+      <c r="K8" s="209">
+        <v>0</v>
+      </c>
+      <c r="L8" s="201">
+        <v>0</v>
+      </c>
+      <c r="M8" s="210">
+        <v>0</v>
+      </c>
+      <c r="N8" s="209">
+        <v>0</v>
+      </c>
+      <c r="O8" s="201">
+        <v>0</v>
+      </c>
+      <c r="P8" s="210">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="150" t="s">
+      <c r="A9" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="203">
-        <v>0</v>
-      </c>
-      <c r="C9" s="204">
-        <v>0</v>
-      </c>
-      <c r="D9" s="212">
-        <v>0</v>
-      </c>
-      <c r="E9" s="203">
-        <v>0</v>
-      </c>
-      <c r="F9" s="204">
-        <v>0</v>
-      </c>
-      <c r="G9" s="212">
-        <v>0</v>
-      </c>
-      <c r="H9" s="203">
-        <v>0</v>
-      </c>
-      <c r="I9" s="204">
-        <v>0</v>
-      </c>
-      <c r="J9" s="212">
-        <v>0</v>
-      </c>
-      <c r="K9" s="203">
-        <v>0</v>
-      </c>
-      <c r="L9" s="204">
-        <v>0</v>
-      </c>
-      <c r="M9" s="212">
-        <v>0</v>
-      </c>
-      <c r="N9" s="203">
-        <v>0</v>
-      </c>
-      <c r="O9" s="204">
-        <v>0</v>
-      </c>
-      <c r="P9" s="212">
+      <c r="B9" s="202">
+        <v>0</v>
+      </c>
+      <c r="C9" s="203">
+        <v>0</v>
+      </c>
+      <c r="D9" s="211">
+        <v>0</v>
+      </c>
+      <c r="E9" s="202">
+        <v>0</v>
+      </c>
+      <c r="F9" s="203">
+        <v>0</v>
+      </c>
+      <c r="G9" s="211">
+        <v>0</v>
+      </c>
+      <c r="H9" s="202">
+        <v>0</v>
+      </c>
+      <c r="I9" s="203">
+        <v>0</v>
+      </c>
+      <c r="J9" s="211">
+        <v>0</v>
+      </c>
+      <c r="K9" s="202">
+        <v>0</v>
+      </c>
+      <c r="L9" s="203">
+        <v>0</v>
+      </c>
+      <c r="M9" s="211">
+        <v>0</v>
+      </c>
+      <c r="N9" s="202">
+        <v>0</v>
+      </c>
+      <c r="O9" s="203">
+        <v>0</v>
+      </c>
+      <c r="P9" s="211">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="203">
-        <v>0</v>
-      </c>
-      <c r="C10" s="204">
-        <v>0</v>
-      </c>
-      <c r="D10" s="212">
-        <v>0</v>
-      </c>
-      <c r="E10" s="203">
-        <v>0</v>
-      </c>
-      <c r="F10" s="204">
-        <v>0</v>
-      </c>
-      <c r="G10" s="212">
-        <v>0</v>
-      </c>
-      <c r="H10" s="203">
+      <c r="B10" s="202">
+        <v>0</v>
+      </c>
+      <c r="C10" s="203">
+        <v>0</v>
+      </c>
+      <c r="D10" s="211">
+        <v>0</v>
+      </c>
+      <c r="E10" s="202">
+        <v>0</v>
+      </c>
+      <c r="F10" s="203">
+        <v>0</v>
+      </c>
+      <c r="G10" s="211">
+        <v>0</v>
+      </c>
+      <c r="H10" s="202">
         <v>1</v>
       </c>
-      <c r="I10" s="204">
-        <v>0</v>
-      </c>
-      <c r="J10" s="212">
-        <v>0</v>
-      </c>
-      <c r="K10" s="203">
-        <v>0</v>
-      </c>
-      <c r="L10" s="204">
-        <v>0</v>
-      </c>
-      <c r="M10" s="212">
-        <v>0</v>
-      </c>
-      <c r="N10" s="203">
-        <v>0</v>
-      </c>
-      <c r="O10" s="204">
-        <v>0</v>
-      </c>
-      <c r="P10" s="212">
+      <c r="I10" s="203">
+        <v>0</v>
+      </c>
+      <c r="J10" s="211">
+        <v>0</v>
+      </c>
+      <c r="K10" s="202">
+        <v>0</v>
+      </c>
+      <c r="L10" s="203">
+        <v>0</v>
+      </c>
+      <c r="M10" s="211">
+        <v>0</v>
+      </c>
+      <c r="N10" s="202">
+        <v>0</v>
+      </c>
+      <c r="O10" s="203">
+        <v>0</v>
+      </c>
+      <c r="P10" s="211">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="198" t="s">
+      <c r="A11" s="197" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="213">
+      <c r="B11" s="212">
         <v>1</v>
       </c>
       <c r="C11" s="102">
         <v>0</v>
       </c>
-      <c r="D11" s="214">
-        <v>0</v>
-      </c>
-      <c r="E11" s="213">
+      <c r="D11" s="213">
+        <v>0</v>
+      </c>
+      <c r="E11" s="212">
         <v>0</v>
       </c>
       <c r="F11" s="102">
         <v>0</v>
       </c>
-      <c r="G11" s="214">
-        <v>0</v>
-      </c>
-      <c r="H11" s="213">
+      <c r="G11" s="213">
+        <v>0</v>
+      </c>
+      <c r="H11" s="212">
         <v>2</v>
       </c>
       <c r="I11" s="102">
         <v>0</v>
       </c>
-      <c r="J11" s="214">
-        <v>0</v>
-      </c>
-      <c r="K11" s="213">
+      <c r="J11" s="213">
+        <v>0</v>
+      </c>
+      <c r="K11" s="212">
         <v>1</v>
       </c>
       <c r="L11" s="102">
         <v>0</v>
       </c>
-      <c r="M11" s="214">
-        <v>0</v>
-      </c>
-      <c r="N11" s="213">
+      <c r="M11" s="213">
+        <v>0</v>
+      </c>
+      <c r="N11" s="212">
         <v>1</v>
       </c>
       <c r="O11" s="102">
         <v>0</v>
       </c>
-      <c r="P11" s="214">
+      <c r="P11" s="213">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="160" t="s">
+      <c r="A12" s="159" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="100">
         <v>1</v>
       </c>
-      <c r="C12" s="215">
-        <v>0</v>
-      </c>
-      <c r="D12" s="216">
+      <c r="C12" s="214">
+        <v>0</v>
+      </c>
+      <c r="D12" s="215">
         <v>0</v>
       </c>
       <c r="E12" s="100">
         <v>0</v>
       </c>
-      <c r="F12" s="215">
-        <v>0</v>
-      </c>
-      <c r="G12" s="216">
+      <c r="F12" s="214">
+        <v>0</v>
+      </c>
+      <c r="G12" s="215">
         <v>0</v>
       </c>
       <c r="H12" s="100">
         <v>0</v>
       </c>
-      <c r="I12" s="215">
-        <v>0</v>
-      </c>
-      <c r="J12" s="216">
+      <c r="I12" s="214">
+        <v>0</v>
+      </c>
+      <c r="J12" s="215">
         <v>0</v>
       </c>
       <c r="K12" s="100">
         <v>2</v>
       </c>
-      <c r="L12" s="215">
-        <v>0</v>
-      </c>
-      <c r="M12" s="216">
+      <c r="L12" s="214">
+        <v>0</v>
+      </c>
+      <c r="M12" s="215">
         <v>0</v>
       </c>
       <c r="N12" s="100">
         <v>2</v>
       </c>
-      <c r="O12" s="215">
-        <v>0</v>
-      </c>
-      <c r="P12" s="216">
+      <c r="O12" s="214">
+        <v>0</v>
+      </c>
+      <c r="P12" s="215">
         <v>0</v>
       </c>
     </row>
@@ -6642,237 +6726,237 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:B12 E3:F7 E10:G12">
-    <cfRule type="cellIs" dxfId="46" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="94" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="45" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12">
-    <cfRule type="cellIs" dxfId="44" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="73" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B7">
-    <cfRule type="cellIs" dxfId="42" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="41" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D7">
-    <cfRule type="cellIs" dxfId="40" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="65" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G7">
-    <cfRule type="cellIs" dxfId="39" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="38" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="37" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="36" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="35" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="34" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="33" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="32" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="31" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="30" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7 H10:I12 K10:K12 N10:N12">
-    <cfRule type="cellIs" dxfId="29" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:J12">
-    <cfRule type="cellIs" dxfId="28" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H7 K3:K7 N3:N7">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="25" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="cellIs" dxfId="24" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9 K9 N9">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="22" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8 K8 N8">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L7 L10:L12">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O7 O10:O12">
-    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:M12">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M7">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10:P12">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P7">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C7 C10:C12">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6927,30 +7011,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="S2" s="239" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="239"/>
-      <c r="U2" s="239"/>
-      <c r="V2" s="239"/>
-      <c r="W2" s="239" t="s">
+      <c r="S2" s="238" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="238"/>
+      <c r="U2" s="238"/>
+      <c r="V2" s="238"/>
+      <c r="W2" s="238" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="239"/>
-      <c r="Y2" s="239"/>
-      <c r="Z2" s="239"/>
-      <c r="AA2" s="239" t="s">
+      <c r="X2" s="238"/>
+      <c r="Y2" s="238"/>
+      <c r="Z2" s="238"/>
+      <c r="AA2" s="238" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="239"/>
-      <c r="AC2" s="239"/>
-      <c r="AD2" s="239"/>
-      <c r="AE2" s="239" t="s">
+      <c r="AB2" s="238"/>
+      <c r="AC2" s="238"/>
+      <c r="AD2" s="238"/>
+      <c r="AE2" s="238" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="239"/>
-      <c r="AG2" s="239"/>
-      <c r="AH2" s="239"/>
+      <c r="AF2" s="238"/>
+      <c r="AG2" s="238"/>
+      <c r="AH2" s="238"/>
       <c r="AK2" s="3" t="s">
         <v>4</v>
       </c>
@@ -8403,10 +8487,10 @@
         <f>1/F17</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J17" s="240" t="s">
+      <c r="J17" s="239" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="243" t="s">
+      <c r="K17" s="242" t="s">
         <v>55</v>
       </c>
       <c r="R17" s="43" t="s">
@@ -8506,8 +8590,8 @@
         <f t="shared" ref="G18:G19" si="9">1/F18</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J18" s="241"/>
-      <c r="K18" s="244"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="243"/>
       <c r="R18" s="46" t="s">
         <v>57</v>
       </c>
@@ -8605,8 +8689,8 @@
         <f t="shared" si="9"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J19" s="241"/>
-      <c r="K19" s="244"/>
+      <c r="J19" s="240"/>
+      <c r="K19" s="243"/>
       <c r="R19" s="46" t="s">
         <v>59</v>
       </c>
@@ -8686,8 +8770,8 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="36"/>
-      <c r="J20" s="241"/>
-      <c r="K20" s="244"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="243"/>
       <c r="R20" s="46" t="s">
         <v>60</v>
       </c>
@@ -8768,8 +8852,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="241"/>
-      <c r="K21" s="244"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="243"/>
       <c r="R21" s="46" t="s">
         <v>61</v>
       </c>
@@ -8850,8 +8934,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="241"/>
-      <c r="K22" s="244"/>
+      <c r="J22" s="240"/>
+      <c r="K22" s="243"/>
       <c r="R22" s="46" t="s">
         <v>62</v>
       </c>
@@ -8932,8 +9016,8 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="241"/>
-      <c r="K23" s="244"/>
+      <c r="J23" s="240"/>
+      <c r="K23" s="243"/>
       <c r="R23" s="48" t="s">
         <v>23</v>
       </c>
@@ -9014,8 +9098,8 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="241"/>
-      <c r="K24" s="244"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="243"/>
       <c r="V24" s="51" t="s">
         <v>63</v>
       </c>
@@ -9036,8 +9120,8 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="241"/>
-      <c r="K25" s="244"/>
+      <c r="J25" s="240"/>
+      <c r="K25" s="243"/>
     </row>
     <row r="26" spans="2:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
@@ -9046,14 +9130,14 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="241"/>
-      <c r="K26" s="244"/>
-      <c r="N26" s="246" t="s">
+      <c r="J26" s="240"/>
+      <c r="K26" s="243"/>
+      <c r="N26" s="245" t="s">
         <v>64</v>
       </c>
-      <c r="O26" s="247"/>
-      <c r="P26" s="247"/>
-      <c r="Q26" s="248"/>
+      <c r="O26" s="246"/>
+      <c r="P26" s="246"/>
+      <c r="Q26" s="247"/>
       <c r="R26" s="52" t="s">
         <v>65</v>
       </c>
@@ -9129,14 +9213,14 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="59"/>
-      <c r="J27" s="241"/>
-      <c r="K27" s="244"/>
-      <c r="N27" s="246" t="s">
+      <c r="J27" s="240"/>
+      <c r="K27" s="243"/>
+      <c r="N27" s="245" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="247"/>
-      <c r="P27" s="247"/>
-      <c r="Q27" s="248"/>
+      <c r="O27" s="246"/>
+      <c r="P27" s="246"/>
+      <c r="Q27" s="247"/>
       <c r="R27" s="55" t="s">
         <v>67</v>
       </c>
@@ -9212,8 +9296,8 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="59"/>
-      <c r="J28" s="241"/>
-      <c r="K28" s="244"/>
+      <c r="J28" s="240"/>
+      <c r="K28" s="243"/>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
@@ -9225,24 +9309,24 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="59"/>
-      <c r="J29" s="241"/>
-      <c r="K29" s="244"/>
+      <c r="J29" s="240"/>
+      <c r="K29" s="243"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J30" s="241"/>
-      <c r="K30" s="244"/>
+      <c r="J30" s="240"/>
+      <c r="K30" s="243"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J31" s="241"/>
-      <c r="K31" s="244"/>
+      <c r="J31" s="240"/>
+      <c r="K31" s="243"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J32" s="241"/>
-      <c r="K32" s="244"/>
+      <c r="J32" s="240"/>
+      <c r="K32" s="243"/>
     </row>
     <row r="33" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J33" s="242"/>
-      <c r="K33" s="245"/>
+      <c r="J33" s="241"/>
+      <c r="K33" s="244"/>
     </row>
     <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U34" s="82"/>
@@ -9354,82 +9438,82 @@
     <mergeCell ref="N27:Q27"/>
   </mergeCells>
   <conditionalFormatting sqref="S5:AB7 AD5:AD7 AD9:AD16 S9:AB16">
-    <cfRule type="cellIs" dxfId="78" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:AD23">
-    <cfRule type="cellIs" dxfId="77" priority="19" operator="notBetween">
+    <cfRule type="cellIs" dxfId="80" priority="19" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="20" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AB8 AD8">
-    <cfRule type="cellIs" dxfId="75" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC5:AC7 AC9:AC16">
-    <cfRule type="cellIs" dxfId="74" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="73" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8">
-    <cfRule type="cellIs" dxfId="72" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5:AF7 AE9:AF16 AH9:AI16 AH5:AJ5 AH6:AI7 AJ6:AJ16 AH4">
-    <cfRule type="cellIs" dxfId="71" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AJ23">
-    <cfRule type="cellIs" dxfId="70" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="73" priority="9" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="72" priority="10" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AF8 AH8:AI8">
-    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5:AG7 AG9:AG16">
-    <cfRule type="cellIs" dxfId="67" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4 S4:AB4">
-    <cfRule type="cellIs" dxfId="66" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AF4 AI4">
-    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
-    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9462,7 +9546,7 @@
         <f>Discretization!B15</f>
         <v>1</v>
       </c>
-      <c r="C1" s="249" t="s">
+      <c r="C1" s="248" t="s">
         <v>261</v>
       </c>
     </row>
@@ -9475,7 +9559,7 @@
         <f>Parameters!B2</f>
         <v>0</v>
       </c>
-      <c r="C2" s="249"/>
+      <c r="C2" s="248"/>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="str">
@@ -9484,31 +9568,31 @@
       </c>
       <c r="B3" s="99" t="str">
         <f>Bacteria!B6</f>
-        <v>granule</v>
-      </c>
-      <c r="C3" s="249"/>
+        <v>suspension</v>
+      </c>
+      <c r="C3" s="248"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="str">
-        <f>Bacteria!A12</f>
+        <f>Bacteria!A13</f>
         <v>Inactivation enabled</v>
       </c>
       <c r="B4" s="99" t="b">
-        <f>Bacteria!B12</f>
+        <f>Bacteria!B13</f>
         <v>1</v>
       </c>
-      <c r="C4" s="249"/>
+      <c r="C4" s="248"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="str">
-        <f>Bacteria!A13</f>
+        <f>Bacteria!A14</f>
         <v>Detachment method</v>
       </c>
       <c r="B5" s="99" t="str">
-        <f>Bacteria!B13</f>
+        <f>Bacteria!B14</f>
         <v>none</v>
       </c>
-      <c r="C5" s="249"/>
+      <c r="C5" s="248"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
@@ -9519,7 +9603,7 @@
         <f>Solver!B4</f>
         <v>1</v>
       </c>
-      <c r="C6" s="249"/>
+      <c r="C6" s="248"/>
     </row>
     <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
@@ -9530,7 +9614,7 @@
         <f>Solver!B2</f>
         <v>0</v>
       </c>
-      <c r="C7" s="249"/>
+      <c r="C7" s="248"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="str">
@@ -9541,32 +9625,32 @@
         <f>Solver!B5</f>
         <v>0</v>
       </c>
-      <c r="C8" s="249"/>
+      <c r="C8" s="248"/>
     </row>
     <row r="9" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="218"/>
-      <c r="G9" s="217"/>
+      <c r="C9" s="217"/>
+      <c r="G9" s="216"/>
     </row>
     <row r="10" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="218"/>
-      <c r="G10" s="217"/>
+      <c r="C10" s="217"/>
+      <c r="G10" s="216"/>
     </row>
     <row r="11" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="218"/>
-      <c r="G11" s="217"/>
+      <c r="C11" s="217"/>
+      <c r="G11" s="216"/>
     </row>
     <row r="12" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="218"/>
-      <c r="G12" s="217"/>
+      <c r="C12" s="217"/>
+      <c r="G12" s="216"/>
     </row>
     <row r="13" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="218"/>
+      <c r="C13" s="217"/>
     </row>
     <row r="14" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="218"/>
+      <c r="C14" s="217"/>
     </row>
     <row r="15" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="218"/>
+      <c r="C15" s="217"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9580,7 +9664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -9606,7 +9690,7 @@
       <c r="D1" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="250" t="s">
+      <c r="E1" s="249" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9623,7 +9707,7 @@
       <c r="D2" s="110" t="s">
         <v>131</v>
       </c>
-      <c r="E2" s="250"/>
+      <c r="E2" s="249"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -9639,7 +9723,7 @@
       <c r="D3" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="250"/>
+      <c r="E3" s="249"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -9655,7 +9739,7 @@
       <c r="D4" s="110" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="250"/>
+      <c r="E4" s="249"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -9670,7 +9754,7 @@
       <c r="D5" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="250"/>
+      <c r="E5" s="249"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -9685,7 +9769,7 @@
       <c r="D6" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="E6" s="250"/>
+      <c r="E6" s="249"/>
     </row>
     <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
@@ -9700,15 +9784,15 @@
       <c r="D7" s="110" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="250"/>
+      <c r="E7" s="249"/>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="89" t="s">
         <v>122</v>
       </c>
       <c r="B8" s="104">
-        <f>20*10^(-6)</f>
-        <v>1.9999999999999998E-5</v>
+        <f>5*10^(-6)</f>
+        <v>4.9999999999999996E-6</v>
       </c>
       <c r="C8" s="92" t="s">
         <v>94</v>
@@ -9716,7 +9800,7 @@
       <c r="D8" s="111" t="s">
         <v>129</v>
       </c>
-      <c r="E8" s="251"/>
+      <c r="E8" s="250"/>
     </row>
     <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
@@ -9731,7 +9815,7 @@
       <c r="D9" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="E9" s="252" t="s">
+      <c r="E9" s="251" t="s">
         <v>138</v>
       </c>
     </row>
@@ -9748,7 +9832,7 @@
       <c r="D10" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="253"/>
+      <c r="E10" s="252"/>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
@@ -9764,7 +9848,7 @@
       <c r="D11" s="110" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="253"/>
+      <c r="E11" s="252"/>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
@@ -9779,7 +9863,7 @@
       <c r="D12" s="110" t="s">
         <v>155</v>
       </c>
-      <c r="E12" s="253"/>
+      <c r="E12" s="252"/>
     </row>
     <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="77" t="s">
@@ -9794,7 +9878,7 @@
       <c r="D13" s="110" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="253"/>
+      <c r="E13" s="252"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="89" t="s">
@@ -9810,7 +9894,7 @@
       <c r="D14" s="111" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="254"/>
+      <c r="E14" s="253"/>
     </row>
     <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="107" t="s">
@@ -9825,7 +9909,7 @@
       <c r="D15" s="113" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="252" t="s">
+      <c r="E15" s="251" t="s">
         <v>173</v>
       </c>
     </row>
@@ -9842,7 +9926,7 @@
       <c r="D16" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="253"/>
+      <c r="E16" s="252"/>
     </row>
     <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="77" t="s">
@@ -9858,7 +9942,7 @@
       <c r="D17" s="114" t="s">
         <v>147</v>
       </c>
-      <c r="E17" s="253"/>
+      <c r="E17" s="252"/>
     </row>
     <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
@@ -9873,7 +9957,7 @@
       <c r="D18" s="114" t="s">
         <v>148</v>
       </c>
-      <c r="E18" s="253"/>
+      <c r="E18" s="252"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
@@ -9889,7 +9973,7 @@
       <c r="D19" s="114" t="s">
         <v>150</v>
       </c>
-      <c r="E19" s="253"/>
+      <c r="E19" s="252"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
@@ -9904,7 +9988,7 @@
       <c r="D20" s="114" t="s">
         <v>156</v>
       </c>
-      <c r="E20" s="253"/>
+      <c r="E20" s="252"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="108" t="s">
@@ -9919,7 +10003,7 @@
       <c r="D21" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="E21" s="253"/>
+      <c r="E21" s="252"/>
     </row>
     <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
@@ -9934,14 +10018,14 @@
       <c r="D22" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="E22" s="253"/>
+      <c r="E22" s="252"/>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
         <v>163</v>
       </c>
       <c r="B23" s="102">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C23" s="127" t="s">
         <v>97</v>
@@ -9949,7 +10033,7 @@
       <c r="D23" s="116" t="s">
         <v>167</v>
       </c>
-      <c r="E23" s="253"/>
+      <c r="E23" s="252"/>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
@@ -9964,7 +10048,7 @@
       <c r="D24" s="116" t="s">
         <v>168</v>
       </c>
-      <c r="E24" s="253"/>
+      <c r="E24" s="252"/>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
@@ -9979,7 +10063,7 @@
       <c r="D25" s="116" t="s">
         <v>169</v>
       </c>
-      <c r="E25" s="253"/>
+      <c r="E25" s="252"/>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="77" t="s">
@@ -9994,14 +10078,15 @@
       <c r="D26" s="116" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="253"/>
+      <c r="E26" s="252"/>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="77" t="s">
         <v>164</v>
       </c>
       <c r="B27" s="118">
-        <v>9.9999999999999995E-7</v>
+        <f>1*10^(-10)</f>
+        <v>1E-10</v>
       </c>
       <c r="C27" s="127" t="s">
         <v>97</v>
@@ -10009,7 +10094,7 @@
       <c r="D27" s="116" t="s">
         <v>171</v>
       </c>
-      <c r="E27" s="253"/>
+      <c r="E27" s="252"/>
     </row>
     <row r="28" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="89" t="s">
@@ -10024,7 +10109,7 @@
       <c r="D28" s="117" t="s">
         <v>172</v>
       </c>
-      <c r="E28" s="254"/>
+      <c r="E28" s="253"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10033,7 +10118,7 @@
     <mergeCell ref="E15:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:D28">
-    <cfRule type="expression" dxfId="62" priority="1">
+    <cfRule type="expression" dxfId="65" priority="1">
       <formula>$B$15 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10052,7 +10137,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D12"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10114,7 +10199,7 @@
       <c r="A4" s="108" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="219" t="s">
+      <c r="B4" s="218" t="s">
         <v>74</v>
       </c>
       <c r="C4" s="126" t="s">
@@ -10144,7 +10229,7 @@
       <c r="A6" s="77" t="s">
         <v>244</v>
       </c>
-      <c r="B6" s="153">
+      <c r="B6" s="152">
         <f>B5+273.15</f>
         <v>293.14999999999998</v>
       </c>
@@ -10160,7 +10245,7 @@
       <c r="A7" s="77" t="s">
         <v>177</v>
       </c>
-      <c r="B7" s="154">
+      <c r="B7" s="153">
         <v>7</v>
       </c>
       <c r="C7" s="90" t="s">
@@ -10177,13 +10262,13 @@
       </c>
       <c r="B8" s="128">
         <f>B11/B12 * 4/3 * PI() *B10^3</f>
-        <v>1.4137166941154067E-9</v>
+        <v>1.1503465099894623E-10</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>98</v>
       </c>
       <c r="D8" s="110" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E8" s="69"/>
     </row>
@@ -10204,47 +10289,47 @@
       <c r="E9" s="69"/>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="220" t="s">
-        <v>281</v>
-      </c>
-      <c r="B10" s="158">
-        <f>150*10^(-6)</f>
-        <v>1.4999999999999999E-4</v>
+      <c r="A10" s="219" t="s">
+        <v>277</v>
+      </c>
+      <c r="B10" s="157">
+        <f>65*10^(-6)</f>
+        <v>6.4999999999999994E-5</v>
       </c>
       <c r="C10" s="90" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="143" t="s">
-        <v>286</v>
+      <c r="D10" s="142" t="s">
+        <v>282</v>
       </c>
       <c r="E10" s="69"/>
     </row>
     <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
-        <v>282</v>
-      </c>
-      <c r="B11" s="236">
+        <v>278</v>
+      </c>
+      <c r="B11" s="234">
         <v>100</v>
       </c>
       <c r="C11" s="90" t="s">
+        <v>280</v>
+      </c>
+      <c r="D11" s="116" t="s">
         <v>284</v>
-      </c>
-      <c r="D11" s="116" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" s="234">
+        <v>1</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>280</v>
+      </c>
+      <c r="D12" s="116" t="s">
         <v>283</v>
-      </c>
-      <c r="B12" s="236">
-        <v>1</v>
-      </c>
-      <c r="C12" s="90" t="s">
-        <v>284</v>
-      </c>
-      <c r="D12" s="116" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -10330,12 +10415,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="61" priority="3">
+    <cfRule type="expression" dxfId="64" priority="3">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="60" priority="1">
+    <cfRule type="expression" dxfId="63" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10384,7 +10469,7 @@
       <c r="D1" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="255" t="s">
+      <c r="E1" s="254" t="s">
         <v>187</v>
       </c>
     </row>
@@ -10402,7 +10487,7 @@
       <c r="D2" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="E2" s="255"/>
+      <c r="E2" s="254"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -10418,7 +10503,7 @@
       <c r="D3" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="E3" s="255"/>
+      <c r="E3" s="254"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -10434,7 +10519,7 @@
       <c r="D4" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="E4" s="255"/>
+      <c r="E4" s="254"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -10450,7 +10535,7 @@
       <c r="D5" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="255"/>
+      <c r="E5" s="254"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -10466,7 +10551,7 @@
       <c r="D6" s="110" t="s">
         <v>186</v>
       </c>
-      <c r="E6" s="255"/>
+      <c r="E6" s="254"/>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="89" t="s">
@@ -10482,7 +10567,7 @@
       <c r="D7" s="111" t="s">
         <v>186</v>
       </c>
-      <c r="E7" s="256"/>
+      <c r="E7" s="255"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10495,10 +10580,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10589,14 +10674,14 @@
       <c r="A6" s="138" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="142" t="s">
-        <v>289</v>
+      <c r="B6" s="237" t="s">
+        <v>287</v>
       </c>
       <c r="C6" s="140" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="141" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
@@ -10616,184 +10701,193 @@
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
-        <v>273</v>
-      </c>
-      <c r="B8" s="230">
-        <f>_xlfn.CEILING.MATH(B7^2 / (0.8*B3 * B11)^2 * 0.75)</f>
+        <v>272</v>
+      </c>
+      <c r="B8" s="132">
+        <f>_xlfn.CEILING.MATH(B7^2 / (0.8*B3 * B12)^2 * 0.75)</f>
         <v>326</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="130" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="108" t="s">
-        <v>274</v>
-      </c>
-      <c r="B9" s="229">
-        <v>200</v>
-      </c>
-      <c r="C9" s="126" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="219" t="s">
+        <v>288</v>
+      </c>
+      <c r="B9" s="132">
+        <v>10</v>
+      </c>
+      <c r="C9" s="265" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="136" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
+      <c r="D9" s="266" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="267" t="s">
+        <v>291</v>
+      </c>
+      <c r="B10" s="264">
+        <v>10</v>
+      </c>
+      <c r="C10" s="126" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="136" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="B10" s="131">
-        <f>ROUND(((B15)^2)/((B3)^2),0)</f>
+      <c r="B11" s="132">
+        <f>ROUND(((B16)^2)/((B3)^2),0)</f>
         <v>64009</v>
-      </c>
-      <c r="C10" s="90" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="130" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="132">
-        <v>1.5</v>
       </c>
       <c r="C11" s="90" t="s">
         <v>97</v>
       </c>
       <c r="D11" s="130" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
-        <v>206</v>
-      </c>
-      <c r="B12" s="137" t="b">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="B12" s="132">
+        <v>1.5</v>
       </c>
       <c r="C12" s="90" t="s">
         <v>97</v>
       </c>
       <c r="D12" s="130" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="137" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="130" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="138" t="s">
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="138" t="s">
         <v>208</v>
       </c>
-      <c r="B13" s="139" t="s">
-        <v>280</v>
-      </c>
-      <c r="C13" s="140" t="s">
+      <c r="B14" s="139" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" s="140" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="141" t="s">
+      <c r="D14" s="141" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="77" t="s">
+    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="77" t="s">
         <v>209</v>
       </c>
-      <c r="B14" s="132">
-        <v>0.5</v>
-      </c>
-      <c r="C14" s="90" t="s">
+      <c r="B15" s="132">
+        <v>0.05</v>
+      </c>
+      <c r="C15" s="90" t="s">
         <v>210</v>
       </c>
-      <c r="D14" s="130" t="s">
+      <c r="D15" s="130" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="108" t="s">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="108" t="s">
         <v>194</v>
       </c>
-      <c r="B15" s="135">
+      <c r="B16" s="135">
         <f>Discretization!B3/2/1000000 - 2*Discretization!B5</f>
         <v>2.5300000000000002E-4</v>
       </c>
-      <c r="C15" s="126" t="s">
+      <c r="C16" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="136" t="s">
+      <c r="D16" s="136" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="69"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="149"/>
-      <c r="C17" s="235"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="94"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="69"/>
-      <c r="D19" s="94"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="148"/>
+      <c r="C18" s="233"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="94"/>
+      <c r="D19" s="69"/>
       <c r="E19" s="69"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="234"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="94"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="237"/>
-      <c r="C21" s="238"/>
+      <c r="D20" s="94"/>
+      <c r="E20" s="69"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="232"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="94"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="235"/>
+      <c r="C22" s="236"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A14:D14">
-    <cfRule type="expression" dxfId="59" priority="5">
-      <formula>$B$13&lt;&gt;"mechanistic"</formula>
+  <conditionalFormatting sqref="A15:D15">
+    <cfRule type="expression" dxfId="7" priority="5">
+      <formula>$B$14&lt;&gt;"mechanistic"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A15:D15 C17">
-    <cfRule type="expression" dxfId="58" priority="4">
-      <formula>$B$13&lt;&gt;"naive"</formula>
+  <conditionalFormatting sqref="A16:D16">
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>$B$14&lt;&gt;"naive"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:D9">
-    <cfRule type="expression" dxfId="57" priority="2">
-      <formula>$B$6 = "granule"</formula>
+  <conditionalFormatting sqref="A9:D10">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>OR($B$6 = "granule", $B$6 = "mature granule")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:D8">
-    <cfRule type="expression" dxfId="56" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$B$6 ="suspension"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="55" priority="1">
-      <formula>$B$13&lt;&gt;"naive"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{4E7A34FD-A1C4-464E-AB3C-F3887798D8D2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{4E7A34FD-A1C4-464E-AB3C-F3887798D8D2}">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{612E5177-E007-4AA1-A867-561F6B98DA27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B14" xr:uid="{612E5177-E007-4AA1-A867-561F6B98DA27}">
       <formula1>"mechanistic, naive, none"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{2612E19F-069C-4D1D-B983-8FF0792C7324}">
-      <formula1>"granule, suspension"</formula1>
+      <formula1>"granule, suspension, mature granule"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10875,7 +10969,7 @@
       <c r="A5" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="B5" s="229" t="b">
+      <c r="B5" s="228" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="126" t="s">
@@ -10903,7 +10997,7 @@
       <c r="A7" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="B7" s="233">
+      <c r="B7" s="231">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C7" s="90" t="s">
@@ -10945,13 +11039,13 @@
       <c r="A10" s="108" t="s">
         <v>229</v>
       </c>
-      <c r="B10" s="229" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="231" t="s">
+      <c r="B10" s="228" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="229" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="232" t="s">
+      <c r="D10" s="230" t="s">
         <v>230</v>
       </c>
     </row>
@@ -10965,7 +11059,7 @@
       <c r="C11" s="127" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="143" t="s">
+      <c r="D11" s="142" t="s">
         <v>258</v>
       </c>
     </row>
@@ -10979,23 +11073,23 @@
       <c r="C12" s="127" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="143" t="s">
+      <c r="D12" s="142" t="s">
         <v>259</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="54" priority="3">
+    <cfRule type="expression" dxfId="62" priority="3">
       <formula>$B$2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:D12">
-    <cfRule type="expression" dxfId="53" priority="2">
+    <cfRule type="expression" dxfId="61" priority="2">
       <formula>$B$11=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D5">
-    <cfRule type="expression" dxfId="52" priority="1">
+    <cfRule type="expression" dxfId="60" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11020,7 +11114,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11036,15 +11130,16 @@
         <v>74</v>
       </c>
       <c r="B1" s="131">
+        <f>500*10^(-6)</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="257" t="s">
+      <c r="E1" s="256" t="s">
         <v>232</v>
       </c>
       <c r="F1" s="69"/>
@@ -11058,15 +11153,16 @@
         <v>75</v>
       </c>
       <c r="B2" s="131">
+        <f>500*10^(-6)</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="144" t="s">
+      <c r="D2" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="257"/>
+      <c r="E2" s="256"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
@@ -11078,15 +11174,16 @@
         <v>80</v>
       </c>
       <c r="B3" s="131">
+        <f t="shared" ref="B3" si="0">500*10^(-6)</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="257"/>
+      <c r="E3" s="256"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
@@ -11104,10 +11201,10 @@
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="144" t="s">
+      <c r="D4" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="257"/>
+      <c r="E4" s="256"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
@@ -11124,10 +11221,10 @@
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="144" t="s">
+      <c r="D5" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="257"/>
+      <c r="E5" s="256"/>
       <c r="F5" s="94"/>
       <c r="G5" s="69"/>
       <c r="H5" s="69"/>
@@ -11145,10 +11242,10 @@
       <c r="C6" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="144" t="s">
+      <c r="D6" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="257"/>
+      <c r="E6" s="256"/>
       <c r="F6" s="94"/>
       <c r="G6" s="69"/>
       <c r="H6" s="69"/>
@@ -11166,10 +11263,10 @@
       <c r="C7" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="144" t="s">
+      <c r="D7" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="257"/>
+      <c r="E7" s="256"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
       <c r="H7" s="69"/>

</xml_diff>

<commit_message>
IbM partial nitrification version
</commit_message>
<xml_diff>
--- a/planning/Excels/Templates/AOBNOBAMXCMX.xlsx
+++ b/planning/Excels/Templates/AOBNOBAMXCMX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bestanden\Cloud Storage\Uni\Master Thesis\version_GitHub\planning\Excels\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2424069M\Documents\GitHub\IbM\planning\Excels\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9556F3C8-4E02-4F81-B5F7-E5F620300B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67CF786-C533-441A-826D-AD296871FE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25080" yWindow="3810" windowWidth="21600" windowHeight="11385" tabRatio="808" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="808" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -29,12 +29,15 @@
     <sheet name="Yield" sheetId="33" r:id="rId14"/>
     <sheet name="ReactionMatrix" sheetId="21" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -51,16 +54,10 @@
   <commentList>
     <comment ref="B11" authorId="0" shapeId="0" xr:uid="{C72CDA48-D953-4720-AEA8-B58D43D4D973}">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Lemaire2008 -&gt; order of magnitude 30-80 g/L for synthetic feed, 150 g/L in their experiment</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -190,7 +187,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Chiel van Amstel:</t>
         </r>
@@ -199,7 +196,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 [mol_x/mol_s]</t>
@@ -208,16 +205,10 @@
     </comment>
     <comment ref="B4" authorId="1" shapeId="0" xr:uid="{C3D489CB-7BCD-4845-B916-FD5651F5211F}">
       <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Average value from literature</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -1534,7 +1525,7 @@
     <t>Residual value of the diffusion equation below which steady state can be assumed. Default: 0.005 mol/L/h</t>
   </si>
   <si>
-    <t>SBR</t>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1542,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1779,6 +1770,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1825,19 +1817,6 @@
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3025,7 +3004,7 @@
     <xf numFmtId="0" fontId="35" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
@@ -3657,6 +3636,7 @@
     <xf numFmtId="11" fontId="0" fillId="11" borderId="77" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3750,7 +3730,35 @@
     <cellStyle name="Percent" xfId="8" builtinId="5"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
@@ -4668,20 +4676,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6616838C-F568-417D-8029-DEFF7E533FF8}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="96" t="s">
         <v>111</v>
       </c>
@@ -4692,7 +4701,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
         <v>118</v>
       </c>
@@ -4703,82 +4712,82 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="69" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="69" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="226" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A10" s="227" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="225" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="224" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A13" s="220" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="219" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A15" s="221" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A16" s="222" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="223" t="s">
         <v>268</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="95" priority="6">
+    <cfRule type="expression" dxfId="99" priority="6">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="containsText" dxfId="94" priority="4" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="98" priority="4" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",A16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="5" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="97" priority="5" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",A16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="92" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="91" priority="1">
+    <cfRule type="expression" dxfId="95" priority="1">
       <formula>$B$11&lt;&gt;"naive"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4789,23 +4798,24 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="62"/>
-    <col min="3" max="3" width="7.5703125" style="62" customWidth="1"/>
-    <col min="4" max="4" width="75.42578125" style="62" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" style="62"/>
+    <col min="1" max="2" width="11.44140625" style="62"/>
+    <col min="3" max="3" width="7.5546875" style="62" customWidth="1"/>
+    <col min="4" max="4" width="75.44140625" style="62" customWidth="1"/>
+    <col min="5" max="6" width="11.44140625" style="62"/>
     <col min="7" max="7" width="12" style="62" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="62"/>
+    <col min="8" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
@@ -4816,14 +4826,14 @@
       <c r="C1" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="262" t="s">
+      <c r="D1" s="263" t="s">
         <v>229</v>
       </c>
       <c r="E1" s="69"/>
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
@@ -4834,12 +4844,12 @@
       <c r="C2" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="262"/>
+      <c r="D2" s="263"/>
       <c r="E2" s="69"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
@@ -4850,12 +4860,12 @@
       <c r="C3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="262"/>
+      <c r="D3" s="263"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
@@ -4866,12 +4876,12 @@
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="262"/>
+      <c r="D4" s="263"/>
       <c r="E4" s="69"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
@@ -4881,12 +4891,12 @@
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="262"/>
+      <c r="D5" s="263"/>
       <c r="E5" s="69"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="108" t="s">
         <v>83</v>
       </c>
@@ -4897,12 +4907,12 @@
       <c r="C6" s="126" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="262"/>
+      <c r="D6" s="263"/>
       <c r="E6" s="69"/>
       <c r="F6" s="69"/>
       <c r="G6" s="69"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="149" t="s">
         <v>84</v>
       </c>
@@ -4912,7 +4922,7 @@
       <c r="C7" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="262"/>
+      <c r="D7" s="263"/>
       <c r="E7" s="69"/>
       <c r="F7" s="144"/>
       <c r="G7" s="144"/>
@@ -4920,7 +4930,7 @@
       <c r="I7" s="145"/>
       <c r="J7" s="145"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="69"/>
       <c r="F8" s="146"/>
       <c r="G8" s="147"/>
@@ -4928,7 +4938,7 @@
       <c r="I8" s="146"/>
       <c r="J8" s="145"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="69"/>
       <c r="B10" s="69"/>
       <c r="C10" s="69"/>
@@ -4937,7 +4947,7 @@
       <c r="F10" s="69"/>
       <c r="G10" s="94"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="69"/>
     </row>
   </sheetData>
@@ -4951,22 +4961,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="6" width="14.28515625" style="75" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="71" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="72" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="6" width="14.33203125" style="75" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="71" customWidth="1"/>
+    <col min="8" max="8" width="3.5546875" style="72" customWidth="1"/>
+    <col min="9" max="9" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="160" t="s">
         <v>91</v>
       </c>
@@ -4989,7 +5000,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>74</v>
       </c>
@@ -5014,11 +5025,11 @@
       <c r="H2" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="262" t="s">
+      <c r="I2" s="263" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>75</v>
       </c>
@@ -5043,9 +5054,9 @@
       <c r="H3" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="262"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I3" s="263"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>80</v>
       </c>
@@ -5070,9 +5081,9 @@
       <c r="H4" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="262"/>
-    </row>
-    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I4" s="263"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>81</v>
       </c>
@@ -5097,9 +5108,9 @@
       <c r="H5" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="262"/>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I5" s="263"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>82</v>
       </c>
@@ -5125,9 +5136,9 @@
       <c r="H6" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="262"/>
-    </row>
-    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I6" s="263"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>83</v>
       </c>
@@ -5154,9 +5165,9 @@
       <c r="H7" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="262"/>
-    </row>
-    <row r="8" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I7" s="263"/>
+    </row>
+    <row r="8" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="149" t="s">
         <v>84</v>
       </c>
@@ -5181,9 +5192,9 @@
       <c r="H8" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="262"/>
-    </row>
-    <row r="9" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I8" s="263"/>
+    </row>
+    <row r="9" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="108" t="s">
         <v>85</v>
       </c>
@@ -5208,9 +5219,9 @@
       <c r="H9" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="262"/>
-    </row>
-    <row r="10" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I9" s="263"/>
+    </row>
+    <row r="10" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="158" t="s">
         <v>86</v>
       </c>
@@ -5235,9 +5246,9 @@
       <c r="H10" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="I10" s="262"/>
-    </row>
-    <row r="11" spans="1:9" s="71" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="263"/>
+    </row>
+    <row r="11" spans="1:9" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="159" t="s">
         <v>18</v>
       </c>
@@ -5262,9 +5273,9 @@
       <c r="H11" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="I11" s="262"/>
-    </row>
-    <row r="12" spans="1:9" s="71" customFormat="1" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="263"/>
+    </row>
+    <row r="12" spans="1:9" s="71" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="160" t="s">
         <v>91</v>
       </c>
@@ -5282,7 +5293,7 @@
       </c>
       <c r="H12" s="72"/>
     </row>
-    <row r="13" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="76" t="s">
         <v>74</v>
       </c>
@@ -5303,11 +5314,11 @@
         <v>0</v>
       </c>
       <c r="H13" s="72"/>
-      <c r="I13" s="261" t="s">
+      <c r="I13" s="262" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>75</v>
       </c>
@@ -5328,9 +5339,9 @@
         <v>0</v>
       </c>
       <c r="H14" s="72"/>
-      <c r="I14" s="261"/>
-    </row>
-    <row r="15" spans="1:9" s="71" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I14" s="262"/>
+    </row>
+    <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>80</v>
       </c>
@@ -5351,9 +5362,9 @@
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="261"/>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I15" s="262"/>
+    </row>
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
         <v>81</v>
       </c>
@@ -5374,9 +5385,9 @@
         <v>0</v>
       </c>
       <c r="F16" s="71"/>
-      <c r="I16" s="261"/>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I16" s="262"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>82</v>
       </c>
@@ -5397,9 +5408,9 @@
         <v>0</v>
       </c>
       <c r="F17" s="71"/>
-      <c r="I17" s="261"/>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I17" s="262"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="108" t="s">
         <v>83</v>
       </c>
@@ -5420,9 +5431,9 @@
       </c>
       <c r="F18" s="71"/>
       <c r="H18" s="71"/>
-      <c r="I18" s="261"/>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I18" s="262"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="149" t="s">
         <v>84</v>
       </c>
@@ -5444,9 +5455,9 @@
       </c>
       <c r="F19" s="71"/>
       <c r="H19" s="71"/>
-      <c r="I19" s="261"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I19" s="262"/>
+    </row>
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="149" t="s">
         <v>85</v>
       </c>
@@ -5468,9 +5479,9 @@
       </c>
       <c r="F20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="261"/>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I20" s="262"/>
+    </row>
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="158" t="s">
         <v>86</v>
       </c>
@@ -5492,9 +5503,9 @@
       </c>
       <c r="F21" s="71"/>
       <c r="H21" s="71"/>
-      <c r="I21" s="261"/>
-    </row>
-    <row r="22" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="262"/>
+    </row>
+    <row r="22" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="159" t="s">
         <v>18</v>
       </c>
@@ -5515,19 +5526,19 @@
         <v>0</v>
       </c>
       <c r="F22" s="71"/>
-      <c r="I22" s="261"/>
-    </row>
-    <row r="23" spans="1:9" ht="28.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="263" t="s">
+      <c r="I22" s="262"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="264" t="s">
         <v>236</v>
       </c>
-      <c r="B23" s="264"/>
-      <c r="C23" s="264"/>
-      <c r="D23" s="264"/>
-      <c r="E23" s="264"/>
-      <c r="F23" s="265"/>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B23" s="265"/>
+      <c r="C23" s="265"/>
+      <c r="D23" s="265"/>
+      <c r="E23" s="265"/>
+      <c r="F23" s="266"/>
+    </row>
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="76" t="s">
         <v>74</v>
       </c>
@@ -5546,11 +5557,11 @@
       <c r="F24" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I24" s="261" t="s">
+      <c r="I24" s="262" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="77" t="s">
         <v>75</v>
       </c>
@@ -5569,9 +5580,9 @@
       <c r="F25" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I25" s="261"/>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I25" s="262"/>
+    </row>
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="77" t="s">
         <v>80</v>
       </c>
@@ -5590,9 +5601,9 @@
       <c r="F26" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I26" s="261"/>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I26" s="262"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
         <v>81</v>
       </c>
@@ -5611,9 +5622,9 @@
       <c r="F27" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I27" s="261"/>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I27" s="262"/>
+    </row>
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
         <v>82</v>
       </c>
@@ -5632,9 +5643,9 @@
       <c r="F28" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I28" s="261"/>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I28" s="262"/>
+    </row>
+    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="108" t="s">
         <v>83</v>
       </c>
@@ -5653,9 +5664,9 @@
       <c r="F29" s="186" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="261"/>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I29" s="262"/>
+    </row>
+    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="149" t="s">
         <v>84</v>
       </c>
@@ -5674,9 +5685,9 @@
       <c r="F30" s="190" t="s">
         <v>93</v>
       </c>
-      <c r="I30" s="261"/>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I30" s="262"/>
+    </row>
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="149" t="s">
         <v>85</v>
       </c>
@@ -5695,9 +5706,9 @@
       <c r="F31" s="188" t="s">
         <v>93</v>
       </c>
-      <c r="I31" s="261"/>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I31" s="262"/>
+    </row>
+    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="158" t="s">
         <v>86</v>
       </c>
@@ -5716,9 +5727,9 @@
       <c r="F32" s="184" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="261"/>
-    </row>
-    <row r="33" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="262"/>
+    </row>
+    <row r="33" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="159" t="s">
         <v>18</v>
       </c>
@@ -5737,7 +5748,7 @@
       <c r="F33" s="173" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="261"/>
+      <c r="I33" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5747,15 +5758,15 @@
     <mergeCell ref="I24:I33"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:F11 B24:F33 B13:E17 B19:E22 B18 D18:E18">
-    <cfRule type="containsText" dxfId="64" priority="54" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="68" priority="54" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Inf">
+    <cfRule type="containsText" dxfId="67" priority="55" operator="containsText" text="Inf">
       <formula>NOT(ISERROR(SEARCH("Inf",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:E17 B19:E22 B18 D18:E18">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5767,23 +5778,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C8F689-441D-42D9-88AF-5DCF32002981}">
+  <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="154" t="s">
         <v>74</v>
@@ -5797,16 +5809,17 @@
       <c r="E1" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="253" t="s">
+      <c r="F1" s="254" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>0.04*10^(-6)</f>
+        <v>4.0000000000000001E-8</v>
       </c>
       <c r="C2" s="155">
         <v>0</v>
@@ -5815,12 +5828,12 @@
         <v>0</v>
       </c>
       <c r="E2" s="155">
-        <f>(0.1/32)/1000</f>
-        <v>3.1250000000000001E-6</v>
-      </c>
-      <c r="F2" s="253"/>
-    </row>
-    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <f>2.6*10^(-6)</f>
+        <v>2.6000000000000001E-6</v>
+      </c>
+      <c r="F2" s="254"/>
+    </row>
+    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>273</v>
       </c>
@@ -5828,41 +5841,45 @@
         <v>0</v>
       </c>
       <c r="C3" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>12.5*10^(-6)</f>
+        <v>1.2499999999999999E-5</v>
       </c>
       <c r="D3" s="155">
         <v>0</v>
       </c>
       <c r="E3" s="155">
-        <f t="shared" ref="E3:E6" si="0">(0.1/32)/1000</f>
-        <v>3.1250000000000001E-6</v>
-      </c>
-      <c r="F3" s="253"/>
-    </row>
-    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <f>2.6*10^(-6)</f>
+        <v>2.6000000000000001E-6</v>
+      </c>
+      <c r="F3" s="254"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
       <c r="B4" s="155">
+        <f>0.06*10^(-6)</f>
+        <v>5.9999999999999995E-8</v>
+      </c>
+      <c r="C4" s="155">
+        <f>1*10^(-6)</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="C4" s="155">
-        <v>9.9999999999999995E-7</v>
-      </c>
       <c r="D4" s="155">
         <v>0</v>
       </c>
       <c r="E4" s="155">
         <v>0</v>
       </c>
-      <c r="F4" s="253"/>
-    </row>
-    <row r="5" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="254"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>119</v>
       </c>
       <c r="B5" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>0.04*10^(-6)</f>
+        <v>4.0000000000000001E-8</v>
       </c>
       <c r="C5" s="155">
         <v>0</v>
@@ -5871,39 +5888,43 @@
         <v>0</v>
       </c>
       <c r="E5" s="155">
-        <f t="shared" si="0"/>
-        <v>3.1250000000000001E-6</v>
-      </c>
-      <c r="F5" s="253"/>
-    </row>
-    <row r="6" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="E5:E6" si="0">2.6*10^(-6)</f>
+        <v>2.6000000000000001E-6</v>
+      </c>
+      <c r="F5" s="254"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>0.04*10^(-6)</f>
+        <v>4.0000000000000001E-8</v>
       </c>
       <c r="C6" s="155">
         <v>0</v>
       </c>
       <c r="D6" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>12.5*10^(-6)</f>
+        <v>1.2499999999999999E-5</v>
       </c>
       <c r="E6" s="155">
         <f t="shared" si="0"/>
-        <v>3.1250000000000001E-6</v>
-      </c>
-      <c r="F6" s="253"/>
-    </row>
-    <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2.6000000000000001E-6</v>
+      </c>
+      <c r="F6" s="254"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="89" t="s">
         <v>289</v>
       </c>
       <c r="B7" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>0.04*10^(-6)</f>
+        <v>4.0000000000000001E-8</v>
       </c>
       <c r="C7" s="155">
-        <v>9.9999999999999995E-7</v>
+        <f>12.5*10^(-6)</f>
+        <v>1.2499999999999999E-5</v>
       </c>
       <c r="D7" s="155">
         <v>0</v>
@@ -5911,20 +5932,40 @@
       <c r="E7" s="155">
         <v>0</v>
       </c>
-      <c r="F7" s="253"/>
+      <c r="F7" s="254"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:F7"/>
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
-  <conditionalFormatting sqref="B2:E6">
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="equal">
+  <conditionalFormatting sqref="B6:C6 B2:E4 B5:D5">
+    <cfRule type="cellIs" dxfId="65" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:E7">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="equal">
+  <conditionalFormatting sqref="D7:E7">
+    <cfRule type="cellIs" dxfId="64" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E6">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5935,21 +5976,22 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6FAE86-699B-425D-9552-4ABBD32F0DFA}">
+  <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="64"/>
       <c r="B1" s="154" t="s">
         <v>74</v>
@@ -5960,11 +6002,11 @@
       <c r="D1" s="154" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="253" t="s">
+      <c r="E1" s="254" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
@@ -5977,9 +6019,9 @@
       <c r="D2" s="155">
         <v>0</v>
       </c>
-      <c r="E2" s="253"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="254"/>
+    </row>
+    <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>273</v>
       </c>
@@ -5992,9 +6034,9 @@
       <c r="D3" s="155">
         <v>0</v>
       </c>
-      <c r="E3" s="253"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="254"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
@@ -6008,9 +6050,9 @@
         <f>0.01*(1/32)*(1/1000)</f>
         <v>3.1250000000000003E-7</v>
       </c>
-      <c r="E4" s="253"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="254"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>119</v>
       </c>
@@ -6023,9 +6065,9 @@
       <c r="D5" s="155">
         <v>0</v>
       </c>
-      <c r="E5" s="253"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="254"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>120</v>
       </c>
@@ -6038,9 +6080,9 @@
       <c r="D6" s="155">
         <v>0</v>
       </c>
-      <c r="E6" s="253"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="254"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="89" t="s">
         <v>289</v>
       </c>
@@ -6053,19 +6095,19 @@
       <c r="D7" s="155">
         <v>0</v>
       </c>
-      <c r="E7" s="253"/>
+      <c r="E7" s="254"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:D6">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:D7">
-    <cfRule type="cellIs" dxfId="58" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6075,23 +6117,24 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765FFA51-252D-42F9-AC75-BD3B676D8AD2}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="73.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="73.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="154" t="s">
         <v>274</v>
       </c>
@@ -6105,7 +6148,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="76" t="s">
         <v>73</v>
       </c>
@@ -6117,16 +6160,17 @@
         <v>74</v>
       </c>
       <c r="D2" s="157">
-        <v>1E-3</v>
+        <f>10%*E2</f>
+        <v>2E-3</v>
       </c>
       <c r="E2" s="241">
-        <v>0.01</v>
-      </c>
-      <c r="F2" s="261" t="s">
+        <v>0.02</v>
+      </c>
+      <c r="F2" s="262" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>273</v>
       </c>
@@ -6137,14 +6181,15 @@
         <v>75</v>
       </c>
       <c r="D3" s="157">
-        <v>1E-3</v>
+        <f t="shared" ref="D3:D7" si="0">10%*E3</f>
+        <v>2E-3</v>
       </c>
       <c r="E3" s="242">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="261"/>
-    </row>
-    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.02</v>
+      </c>
+      <c r="F3" s="262"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
@@ -6155,14 +6200,15 @@
         <v>74</v>
       </c>
       <c r="D4" s="157">
-        <v>1E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E4" s="242">
-        <v>0.01</v>
-      </c>
-      <c r="F4" s="261"/>
-    </row>
-    <row r="5" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F4" s="262"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>119</v>
       </c>
@@ -6173,14 +6219,15 @@
         <v>74</v>
       </c>
       <c r="D5" s="157">
-        <v>1E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E5" s="242">
-        <v>0.01</v>
-      </c>
-      <c r="F5" s="261"/>
-    </row>
-    <row r="6" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F5" s="262"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>120</v>
       </c>
@@ -6191,14 +6238,15 @@
         <v>80</v>
       </c>
       <c r="D6" s="157">
-        <v>1E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E6" s="242">
-        <v>0.01</v>
-      </c>
-      <c r="F6" s="261"/>
-    </row>
-    <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F6" s="262"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="89" t="s">
         <v>289</v>
       </c>
@@ -6209,12 +6257,13 @@
         <v>74</v>
       </c>
       <c r="D7" s="157">
-        <v>1E-3</v>
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E7" s="242">
-        <v>0.01</v>
-      </c>
-      <c r="F7" s="261"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F7" s="262"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6227,6 +6276,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6237,52 +6287,52 @@
       <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="62" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="62" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="62" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="62" customWidth="1"/>
     <col min="3" max="3" width="13" style="62" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="62" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="62" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="62" customWidth="1"/>
     <col min="6" max="6" width="14" style="62" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="62" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="62"/>
+    <col min="7" max="7" width="16.88671875" style="62" customWidth="1"/>
+    <col min="8" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
-      <c r="B1" s="268" t="s">
+      <c r="B1" s="269" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="266"/>
-      <c r="D1" s="267"/>
-      <c r="E1" s="268" t="s">
+      <c r="C1" s="267"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="269" t="s">
         <v>273</v>
       </c>
-      <c r="F1" s="266"/>
-      <c r="G1" s="267"/>
-      <c r="H1" s="266" t="s">
+      <c r="F1" s="267"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="267" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="266"/>
-      <c r="J1" s="267"/>
-      <c r="K1" s="266" t="s">
+      <c r="I1" s="267"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="267" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="266"/>
-      <c r="M1" s="267"/>
-      <c r="N1" s="266" t="s">
+      <c r="L1" s="267"/>
+      <c r="M1" s="268"/>
+      <c r="N1" s="267" t="s">
         <v>120</v>
       </c>
-      <c r="O1" s="266"/>
-      <c r="P1" s="267"/>
-      <c r="Q1" s="266" t="s">
+      <c r="O1" s="267"/>
+      <c r="P1" s="268"/>
+      <c r="Q1" s="267" t="s">
         <v>289</v>
       </c>
-      <c r="R1" s="266"/>
-      <c r="S1" s="267"/>
-    </row>
-    <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="267"/>
+      <c r="S1" s="268"/>
+    </row>
+    <row r="2" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
       <c r="B2" s="198" t="s">
         <v>77</v>
@@ -6339,7 +6389,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>74</v>
       </c>
@@ -6398,7 +6448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>75</v>
       </c>
@@ -6457,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>80</v>
       </c>
@@ -6516,7 +6566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>81</v>
       </c>
@@ -6575,7 +6625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>82</v>
       </c>
@@ -6634,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>83</v>
       </c>
@@ -6693,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="149" t="s">
         <v>84</v>
       </c>
@@ -6752,7 +6802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="149" t="s">
         <v>85</v>
       </c>
@@ -6811,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="197" t="s">
         <v>86</v>
       </c>
@@ -6870,7 +6920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="159" t="s">
         <v>18</v>
       </c>
@@ -6939,292 +6989,292 @@
     <mergeCell ref="K1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="B10:B12 E3:F7 E10:G12">
-    <cfRule type="cellIs" dxfId="57" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="105" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="56" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="71" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D12">
-    <cfRule type="cellIs" dxfId="55" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="84" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="54" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B7">
-    <cfRule type="cellIs" dxfId="53" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="78" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="52" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="77" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D7">
-    <cfRule type="cellIs" dxfId="51" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="76" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G7">
-    <cfRule type="cellIs" dxfId="50" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="49" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="69" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="48" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="47" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="65" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="cellIs" dxfId="46" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="cellIs" dxfId="45" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="cellIs" dxfId="44" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="61" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="43" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="42" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="cellIs" dxfId="41" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I7 H10:I12 K10:K12 N10:N12">
-    <cfRule type="cellIs" dxfId="40" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:J12">
-    <cfRule type="cellIs" dxfId="39" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H7 K3:K7 N3:N7">
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3">
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J7">
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9 K9 N9">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8 K8 N8">
-    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L7 L10:L12">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9">
-    <cfRule type="cellIs" dxfId="28" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O7 O10:O12">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O9">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O8">
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:M12">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3">
-    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M7">
-    <cfRule type="cellIs" dxfId="20" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10:P12">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3">
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P7">
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C7 C10:C12">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R7 Q10:R12">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S10:S12">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:Q7">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S3">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S4:S7">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q9">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R9">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q8">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7235,7 +7285,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="B2:AN39"/>
@@ -7244,65 +7294,65 @@
       <selection activeCell="I3" sqref="I3:I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="8" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="15" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="1" customWidth="1"/>
-    <col min="13" max="14" width="4.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4.88671875" style="1" customWidth="1"/>
+    <col min="13" max="14" width="4.44140625" style="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="1" customWidth="1"/>
-    <col min="16" max="17" width="4.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="1" customWidth="1"/>
-    <col min="19" max="20" width="12.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="12.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="1" customWidth="1"/>
-    <col min="27" max="28" width="12.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="15.5703125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="12.42578125" style="1" customWidth="1"/>
-    <col min="31" max="32" width="12.5703125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="15.5703125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.42578125" style="1" customWidth="1"/>
-    <col min="35" max="36" width="8.85546875" style="1"/>
-    <col min="37" max="37" width="14.85546875" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.85546875" style="1"/>
+    <col min="16" max="17" width="4.5546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.44140625" style="1" customWidth="1"/>
+    <col min="19" max="20" width="12.88671875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" style="1" customWidth="1"/>
+    <col min="23" max="24" width="12.44140625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.44140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.44140625" style="1" customWidth="1"/>
+    <col min="27" max="28" width="12.5546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.5546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.44140625" style="1" customWidth="1"/>
+    <col min="31" max="32" width="12.5546875" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" style="1" customWidth="1"/>
+    <col min="35" max="36" width="8.88671875" style="1"/>
+    <col min="37" max="37" width="14.88671875" style="1" customWidth="1"/>
+    <col min="38" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S2" s="243" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="243"/>
-      <c r="U2" s="243"/>
-      <c r="V2" s="243"/>
-      <c r="W2" s="243" t="s">
+    <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="244" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="244"/>
+      <c r="U2" s="244"/>
+      <c r="V2" s="244"/>
+      <c r="W2" s="244" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="243"/>
-      <c r="Y2" s="243"/>
-      <c r="Z2" s="243"/>
-      <c r="AA2" s="243" t="s">
+      <c r="X2" s="244"/>
+      <c r="Y2" s="244"/>
+      <c r="Z2" s="244"/>
+      <c r="AA2" s="244" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="243"/>
-      <c r="AC2" s="243"/>
-      <c r="AD2" s="243"/>
-      <c r="AE2" s="243" t="s">
+      <c r="AB2" s="244"/>
+      <c r="AC2" s="244"/>
+      <c r="AD2" s="244"/>
+      <c r="AE2" s="244" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="243"/>
-      <c r="AG2" s="243"/>
-      <c r="AH2" s="243"/>
+      <c r="AF2" s="244"/>
+      <c r="AG2" s="244"/>
+      <c r="AH2" s="244"/>
       <c r="AK2" s="3" t="s">
         <v>4</v>
       </c>
@@ -7316,7 +7366,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
@@ -7430,7 +7480,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -7525,7 +7575,7 @@
       <c r="AM4" s="19"/>
       <c r="AN4" s="19"/>
     </row>
-    <row r="5" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B5" s="20" t="s">
         <v>33</v>
       </c>
@@ -7648,7 +7698,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
@@ -7772,7 +7822,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="B7" s="20" t="s">
         <v>42</v>
       </c>
@@ -7887,7 +7937,7 @@
       <c r="AM7" s="27"/>
       <c r="AN7" s="27"/>
     </row>
-    <row r="8" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B8" s="20" t="s">
         <v>3</v>
       </c>
@@ -7999,7 +8049,7 @@
       </c>
       <c r="AJ8" s="87"/>
     </row>
-    <row r="9" spans="2:40" ht="20.25" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:40" ht="19.2" x14ac:dyDescent="0.4">
       <c r="I9" s="35" t="s">
         <v>45</v>
       </c>
@@ -8089,7 +8139,7 @@
       </c>
       <c r="AJ9" s="87"/>
     </row>
-    <row r="10" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="I10" s="35" t="s">
         <v>46</v>
       </c>
@@ -8174,7 +8224,7 @@
       </c>
       <c r="AJ10" s="87"/>
     </row>
-    <row r="11" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="I11" s="35" t="s">
         <v>47</v>
       </c>
@@ -8260,7 +8310,7 @@
       </c>
       <c r="AJ11" s="87"/>
     </row>
-    <row r="12" spans="2:40" ht="19.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:40" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="I12" s="35" t="s">
         <v>48</v>
       </c>
@@ -8346,7 +8396,7 @@
       </c>
       <c r="AJ12" s="87"/>
     </row>
-    <row r="13" spans="2:40" ht="21.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:40" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="B13" s="61" t="s">
         <v>49</v>
       </c>
@@ -8442,7 +8492,7 @@
       </c>
       <c r="AJ13" s="87"/>
     </row>
-    <row r="14" spans="2:40" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:40" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" s="31"/>
       <c r="E14" s="34"/>
       <c r="I14" s="29" t="s">
@@ -8532,7 +8582,7 @@
       </c>
       <c r="AJ14" s="87"/>
     </row>
-    <row r="15" spans="2:40" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:40" ht="18" x14ac:dyDescent="0.3">
       <c r="B15" s="31"/>
       <c r="E15" s="34"/>
       <c r="I15" s="29" t="s">
@@ -8624,7 +8674,7 @@
       </c>
       <c r="AJ15" s="87"/>
     </row>
-    <row r="16" spans="2:40" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:40" ht="19.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="6" t="s">
         <v>8</v>
       </c>
@@ -8732,7 +8782,7 @@
       </c>
       <c r="AJ16" s="87"/>
     </row>
-    <row r="17" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="20" t="s">
         <v>33</v>
       </c>
@@ -8755,10 +8805,10 @@
         <f>1/F17</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J17" s="244" t="s">
+      <c r="J17" s="245" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="247" t="s">
+      <c r="K17" s="248" t="s">
         <v>55</v>
       </c>
       <c r="R17" s="43" t="s">
@@ -8834,7 +8884,7 @@
       </c>
       <c r="AJ17" s="27"/>
     </row>
-    <row r="18" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="20" t="s">
         <v>1</v>
       </c>
@@ -8858,8 +8908,8 @@
         <f t="shared" ref="G18:G19" si="9">1/F18</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J18" s="245"/>
-      <c r="K18" s="248"/>
+      <c r="J18" s="246"/>
+      <c r="K18" s="249"/>
       <c r="R18" s="46" t="s">
         <v>57</v>
       </c>
@@ -8933,7 +8983,7 @@
       </c>
       <c r="AJ18" s="27"/>
     </row>
-    <row r="19" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="20" t="s">
         <v>58</v>
       </c>
@@ -8957,8 +9007,8 @@
         <f t="shared" si="9"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J19" s="245"/>
-      <c r="K19" s="248"/>
+      <c r="J19" s="246"/>
+      <c r="K19" s="249"/>
       <c r="R19" s="46" t="s">
         <v>59</v>
       </c>
@@ -9032,14 +9082,14 @@
       </c>
       <c r="AJ19" s="27"/>
     </row>
-    <row r="20" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="58"/>
       <c r="C20" s="58"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="36"/>
-      <c r="J20" s="245"/>
-      <c r="K20" s="248"/>
+      <c r="J20" s="246"/>
+      <c r="K20" s="249"/>
       <c r="R20" s="46" t="s">
         <v>60</v>
       </c>
@@ -9113,15 +9163,15 @@
       </c>
       <c r="AJ20" s="27"/>
     </row>
-    <row r="21" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="58"/>
       <c r="C21" s="58"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="245"/>
-      <c r="K21" s="248"/>
+      <c r="J21" s="246"/>
+      <c r="K21" s="249"/>
       <c r="R21" s="46" t="s">
         <v>61</v>
       </c>
@@ -9195,15 +9245,15 @@
       </c>
       <c r="AJ21" s="27"/>
     </row>
-    <row r="22" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="58"/>
       <c r="C22" s="58"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="245"/>
-      <c r="K22" s="248"/>
+      <c r="J22" s="246"/>
+      <c r="K22" s="249"/>
       <c r="R22" s="46" t="s">
         <v>62</v>
       </c>
@@ -9277,15 +9327,15 @@
       </c>
       <c r="AJ22" s="27"/>
     </row>
-    <row r="23" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="58"/>
       <c r="C23" s="58"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="245"/>
-      <c r="K23" s="248"/>
+      <c r="J23" s="246"/>
+      <c r="K23" s="249"/>
       <c r="R23" s="48" t="s">
         <v>23</v>
       </c>
@@ -9359,15 +9409,15 @@
       </c>
       <c r="AJ23" s="27"/>
     </row>
-    <row r="24" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="58"/>
       <c r="C24" s="58"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="245"/>
-      <c r="K24" s="248"/>
+      <c r="J24" s="246"/>
+      <c r="K24" s="249"/>
       <c r="V24" s="51" t="s">
         <v>63</v>
       </c>
@@ -9381,31 +9431,31 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="58"/>
       <c r="C25" s="58"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="245"/>
-      <c r="K25" s="248"/>
-    </row>
-    <row r="26" spans="2:36" ht="18" x14ac:dyDescent="0.25">
+      <c r="J25" s="246"/>
+      <c r="K25" s="249"/>
+    </row>
+    <row r="26" spans="2:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
       <c r="C26" s="58"/>
       <c r="D26" s="19"/>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="245"/>
-      <c r="K26" s="248"/>
-      <c r="N26" s="250" t="s">
+      <c r="J26" s="246"/>
+      <c r="K26" s="249"/>
+      <c r="N26" s="251" t="s">
         <v>64</v>
       </c>
-      <c r="O26" s="251"/>
-      <c r="P26" s="251"/>
-      <c r="Q26" s="252"/>
+      <c r="O26" s="252"/>
+      <c r="P26" s="252"/>
+      <c r="Q26" s="253"/>
       <c r="R26" s="52" t="s">
         <v>65</v>
       </c>
@@ -9474,21 +9524,21 @@
         <v>263.94800000000009</v>
       </c>
     </row>
-    <row r="27" spans="2:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="58"/>
       <c r="C27" s="58"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="59"/>
-      <c r="J27" s="245"/>
-      <c r="K27" s="248"/>
-      <c r="N27" s="250" t="s">
+      <c r="J27" s="246"/>
+      <c r="K27" s="249"/>
+      <c r="N27" s="251" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="251"/>
-      <c r="P27" s="251"/>
-      <c r="Q27" s="252"/>
+      <c r="O27" s="252"/>
+      <c r="P27" s="252"/>
+      <c r="Q27" s="253"/>
       <c r="R27" s="55" t="s">
         <v>67</v>
       </c>
@@ -9557,46 +9607,46 @@
         <v>303.90184335522252</v>
       </c>
     </row>
-    <row r="28" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="58"/>
       <c r="C28" s="58"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="59"/>
-      <c r="J28" s="245"/>
-      <c r="K28" s="248"/>
+      <c r="J28" s="246"/>
+      <c r="K28" s="249"/>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
     </row>
-    <row r="29" spans="2:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="58"/>
       <c r="C29" s="58"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="59"/>
-      <c r="J29" s="245"/>
-      <c r="K29" s="248"/>
-    </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="J30" s="245"/>
-      <c r="K30" s="248"/>
-    </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="J31" s="245"/>
-      <c r="K31" s="248"/>
-    </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="J32" s="245"/>
-      <c r="K32" s="248"/>
-    </row>
-    <row r="33" spans="10:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J33" s="246"/>
-      <c r="K33" s="249"/>
-    </row>
-    <row r="34" spans="10:26" x14ac:dyDescent="0.25">
+      <c r="J29" s="246"/>
+      <c r="K29" s="249"/>
+    </row>
+    <row r="30" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="J30" s="246"/>
+      <c r="K30" s="249"/>
+    </row>
+    <row r="31" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="J31" s="246"/>
+      <c r="K31" s="249"/>
+    </row>
+    <row r="32" spans="2:36" x14ac:dyDescent="0.3">
+      <c r="J32" s="246"/>
+      <c r="K32" s="249"/>
+    </row>
+    <row r="33" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J33" s="247"/>
+      <c r="K33" s="250"/>
+    </row>
+    <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U34" s="82"/>
       <c r="V34" s="65">
         <v>10</v>
@@ -9610,7 +9660,7 @@
       <c r="Y34"/>
       <c r="Z34"/>
     </row>
-    <row r="35" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U35" s="83" t="s">
         <v>68</v>
       </c>
@@ -9629,7 +9679,7 @@
       <c r="Y35"/>
       <c r="Z35"/>
     </row>
-    <row r="36" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U36" s="84" t="s">
         <v>69</v>
       </c>
@@ -9648,7 +9698,7 @@
       <c r="Y36"/>
       <c r="Z36"/>
     </row>
-    <row r="37" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U37" s="83" t="s">
         <v>70</v>
       </c>
@@ -9667,7 +9717,7 @@
       <c r="Y37"/>
       <c r="Z37"/>
     </row>
-    <row r="38" spans="10:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U38" s="85" t="s">
         <v>71</v>
       </c>
@@ -9686,7 +9736,7 @@
       <c r="Y38"/>
       <c r="Z38"/>
     </row>
-    <row r="39" spans="10:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U39"/>
       <c r="V39"/>
       <c r="W39"/>
@@ -9706,82 +9756,82 @@
     <mergeCell ref="N27:Q27"/>
   </mergeCells>
   <conditionalFormatting sqref="S5:AB7 AD5:AD7 AD9:AD16 S9:AB16">
-    <cfRule type="cellIs" dxfId="90" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S17:AD23">
-    <cfRule type="cellIs" dxfId="89" priority="19" operator="notBetween">
+    <cfRule type="cellIs" dxfId="93" priority="19" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="92" priority="20" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S8:AB8 AD8">
-    <cfRule type="cellIs" dxfId="87" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC5:AC7 AC9:AC16">
-    <cfRule type="cellIs" dxfId="86" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="85" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG8">
-    <cfRule type="cellIs" dxfId="84" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE5:AF7 AE9:AF16 AH9:AI16 AH5:AJ5 AH6:AI7 AJ6:AJ16 AH4">
-    <cfRule type="cellIs" dxfId="83" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AJ23">
-    <cfRule type="cellIs" dxfId="82" priority="9" operator="notBetween">
+    <cfRule type="cellIs" dxfId="86" priority="9" operator="notBetween">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="85" priority="10" operator="between">
       <formula>0.0000000001</formula>
       <formula>-0.0000000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AF8 AH8:AI8">
-    <cfRule type="cellIs" dxfId="80" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG5:AG7 AG9:AG16">
-    <cfRule type="cellIs" dxfId="79" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4 S4:AB4">
-    <cfRule type="cellIs" dxfId="78" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4">
-    <cfRule type="cellIs" dxfId="77" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AF4 AI4">
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4">
-    <cfRule type="cellIs" dxfId="75" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9792,20 +9842,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC80DB5-92D9-44E1-984F-05E418326CA4}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="str">
         <f>Discretization!A15</f>
         <v>Dynamic dT</v>
@@ -9814,11 +9865,11 @@
         <f>Discretization!B15</f>
         <v>1</v>
       </c>
-      <c r="C1" s="253" t="s">
+      <c r="C1" s="254" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="str">
         <f>Parameters!A2</f>
         <v>Variable HRT</v>
@@ -9827,9 +9878,9 @@
         <f>Parameters!B2</f>
         <v>0</v>
       </c>
-      <c r="C2" s="253"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C2" s="254"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="str">
         <f>Bacteria!A6</f>
         <v>Initialisation method</v>
@@ -9838,9 +9889,9 @@
         <f>Bacteria!B6</f>
         <v>suspension</v>
       </c>
-      <c r="C3" s="253"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C3" s="254"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="str">
         <f>Bacteria!A13</f>
         <v>Inactivation enabled</v>
@@ -9849,20 +9900,20 @@
         <f>Bacteria!B13</f>
         <v>1</v>
       </c>
-      <c r="C4" s="253"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C4" s="254"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="str">
         <f>Bacteria!A14</f>
         <v>Detachment method</v>
       </c>
       <c r="B5" s="99" t="str">
         <f>Bacteria!B14</f>
-        <v>SBR</v>
-      </c>
-      <c r="C5" s="253"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>none</v>
+      </c>
+      <c r="C5" s="254"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
         <f>Solver!A4</f>
         <v>pH bulk concentration corrected</v>
@@ -9871,9 +9922,9 @@
         <f>Solver!B4</f>
         <v>1</v>
       </c>
-      <c r="C6" s="253"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="C6" s="254"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
         <f>Solver!A2</f>
         <v>pH solving included</v>
@@ -9882,9 +9933,9 @@
         <f>Solver!B2</f>
         <v>0</v>
       </c>
-      <c r="C7" s="253"/>
-    </row>
-    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="254"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="str">
         <f>Solver!A5</f>
         <v>Speciation included</v>
@@ -9893,31 +9944,31 @@
         <f>Solver!B5</f>
         <v>0</v>
       </c>
-      <c r="C8" s="253"/>
-    </row>
-    <row r="9" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="254"/>
+    </row>
+    <row r="9" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="217"/>
       <c r="G9" s="216"/>
     </row>
-    <row r="10" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="217"/>
       <c r="G10" s="216"/>
     </row>
-    <row r="11" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="217"/>
       <c r="G11" s="216"/>
     </row>
-    <row r="12" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="217"/>
       <c r="G12" s="216"/>
     </row>
-    <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="217"/>
     </row>
-    <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="217"/>
     </row>
-    <row r="15" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="217"/>
     </row>
   </sheetData>
@@ -9930,23 +9981,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="62"/>
-    <col min="4" max="4" width="66.85546875" style="62" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="1" width="33.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="66.88671875" style="62" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>101</v>
       </c>
@@ -9959,11 +10011,11 @@
       <c r="D1" s="110" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="254" t="s">
+      <c r="E1" s="255" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>102</v>
       </c>
@@ -9976,9 +10028,9 @@
       <c r="D2" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="254"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E2" s="255"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
         <v>103</v>
       </c>
@@ -9992,9 +10044,9 @@
       <c r="D3" s="110" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="254"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E3" s="255"/>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
         <v>104</v>
       </c>
@@ -10008,9 +10060,9 @@
       <c r="D4" s="110" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="254"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E4" s="255"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>105</v>
       </c>
@@ -10023,9 +10075,9 @@
       <c r="D5" s="110" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="254"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E5" s="255"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
         <v>106</v>
       </c>
@@ -10038,9 +10090,9 @@
       <c r="D6" s="110" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="254"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E6" s="255"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
         <v>107</v>
       </c>
@@ -10054,9 +10106,9 @@
       <c r="D7" s="110" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="254"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="255"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="89" t="s">
         <v>121</v>
       </c>
@@ -10070,9 +10122,9 @@
       <c r="D8" s="111" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="255"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="256"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
         <v>138</v>
       </c>
@@ -10085,11 +10137,11 @@
       <c r="D9" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="E9" s="256" t="s">
+      <c r="E9" s="257" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="77" t="s">
         <v>141</v>
       </c>
@@ -10102,9 +10154,9 @@
       <c r="D10" s="110" t="s">
         <v>148</v>
       </c>
-      <c r="E10" s="257"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E10" s="258"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
         <v>144</v>
       </c>
@@ -10118,9 +10170,9 @@
       <c r="D11" s="110" t="s">
         <v>150</v>
       </c>
-      <c r="E11" s="257"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E11" s="258"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
         <v>153</v>
       </c>
@@ -10133,9 +10185,9 @@
       <c r="D12" s="110" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="257"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E12" s="258"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="77" t="s">
         <v>132</v>
       </c>
@@ -10148,15 +10200,15 @@
       <c r="D13" s="110" t="s">
         <v>134</v>
       </c>
-      <c r="E13" s="257"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="258"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="89" t="s">
         <v>133</v>
       </c>
       <c r="B14" s="100">
-        <f>7*B13</f>
-        <v>672</v>
+        <f>B13</f>
+        <v>96</v>
       </c>
       <c r="C14" s="124" t="s">
         <v>100</v>
@@ -10164,9 +10216,9 @@
       <c r="D14" s="111" t="s">
         <v>135</v>
       </c>
-      <c r="E14" s="258"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" s="259"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="107" t="s">
         <v>157</v>
       </c>
@@ -10179,11 +10231,11 @@
       <c r="D15" s="113" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="256" t="s">
+      <c r="E15" s="257" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="77" t="s">
         <v>139</v>
       </c>
@@ -10196,9 +10248,9 @@
       <c r="D16" s="114" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="257"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E16" s="258"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="77" t="s">
         <v>142</v>
       </c>
@@ -10212,9 +10264,9 @@
       <c r="D17" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="257"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E17" s="258"/>
+    </row>
+    <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
         <v>140</v>
       </c>
@@ -10227,9 +10279,9 @@
       <c r="D18" s="114" t="s">
         <v>147</v>
       </c>
-      <c r="E18" s="257"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E18" s="258"/>
+    </row>
+    <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
         <v>143</v>
       </c>
@@ -10243,9 +10295,9 @@
       <c r="D19" s="114" t="s">
         <v>149</v>
       </c>
-      <c r="E19" s="257"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E19" s="258"/>
+    </row>
+    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
         <v>151</v>
       </c>
@@ -10258,9 +10310,9 @@
       <c r="D20" s="114" t="s">
         <v>155</v>
       </c>
-      <c r="E20" s="257"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E20" s="258"/>
+    </row>
+    <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="108" t="s">
         <v>152</v>
       </c>
@@ -10273,9 +10325,9 @@
       <c r="D21" s="115" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="257"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" s="258"/>
+    </row>
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="77" t="s">
         <v>159</v>
       </c>
@@ -10288,9 +10340,9 @@
       <c r="D22" s="116" t="s">
         <v>165</v>
       </c>
-      <c r="E22" s="257"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E22" s="258"/>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
         <v>162</v>
       </c>
@@ -10303,9 +10355,9 @@
       <c r="D23" s="116" t="s">
         <v>166</v>
       </c>
-      <c r="E23" s="257"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E23" s="258"/>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
         <v>160</v>
       </c>
@@ -10318,9 +10370,9 @@
       <c r="D24" s="116" t="s">
         <v>167</v>
       </c>
-      <c r="E24" s="257"/>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E24" s="258"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
         <v>161</v>
       </c>
@@ -10333,9 +10385,9 @@
       <c r="D25" s="116" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="257"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E25" s="258"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="77" t="s">
         <v>169</v>
       </c>
@@ -10348,9 +10400,9 @@
       <c r="D26" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="E26" s="257"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" s="258"/>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="77" t="s">
         <v>163</v>
       </c>
@@ -10364,9 +10416,9 @@
       <c r="D27" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="257"/>
-    </row>
-    <row r="28" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="258"/>
+    </row>
+    <row r="28" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="89" t="s">
         <v>164</v>
       </c>
@@ -10379,7 +10431,7 @@
       <c r="D28" s="117" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="258"/>
+      <c r="E28" s="259"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10388,7 +10440,7 @@
     <mergeCell ref="E15:E28"/>
   </mergeCells>
   <conditionalFormatting sqref="A16:D28">
-    <cfRule type="expression" dxfId="74" priority="1">
+    <cfRule type="expression" dxfId="78" priority="1">
       <formula>$B$15 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10404,22 +10456,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" style="62" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="62"/>
+    <col min="1" max="1" width="21.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="62" customWidth="1"/>
+    <col min="4" max="4" width="69.44140625" style="62" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>99</v>
       </c>
@@ -10434,7 +10487,7 @@
       </c>
       <c r="E1" s="69"/>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>177</v>
       </c>
@@ -10449,7 +10502,7 @@
       </c>
       <c r="E2" s="69"/>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
         <v>180</v>
       </c>
@@ -10465,7 +10518,7 @@
       </c>
       <c r="E3" s="69"/>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="108" t="s">
         <v>181</v>
       </c>
@@ -10480,7 +10533,7 @@
       </c>
       <c r="E4" s="69"/>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>39</v>
       </c>
@@ -10495,7 +10548,7 @@
       </c>
       <c r="E5" s="69"/>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
         <v>242</v>
       </c>
@@ -10511,7 +10564,7 @@
       </c>
       <c r="E6" s="69"/>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
         <v>176</v>
       </c>
@@ -10526,7 +10579,7 @@
       </c>
       <c r="E7" s="69"/>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="77" t="s">
         <v>175</v>
       </c>
@@ -10542,7 +10595,7 @@
       </c>
       <c r="E8" s="69"/>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="77" t="s">
         <v>174</v>
       </c>
@@ -10558,7 +10611,7 @@
       </c>
       <c r="E9" s="69"/>
     </row>
-    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="219" t="s">
         <v>275</v>
       </c>
@@ -10574,7 +10627,7 @@
       </c>
       <c r="E10" s="69"/>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
         <v>287</v>
       </c>
@@ -10588,7 +10641,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
         <v>288</v>
       </c>
@@ -10602,95 +10655,95 @@
         <v>279</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14"/>
-      <c r="B14"/>
+      <c r="B14" s="243"/>
       <c r="C14"/>
       <c r="D14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" s="94"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="69"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="73" priority="3">
+    <cfRule type="expression" dxfId="77" priority="3">
       <formula>$B$2 = FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1">
-    <cfRule type="expression" dxfId="72" priority="1">
+    <cfRule type="expression" dxfId="76" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10707,25 +10760,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="62"/>
+    <col min="1" max="1" width="9.109375" style="62"/>
     <col min="2" max="2" width="12" style="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="62" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="62" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="62" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="62"/>
-    <col min="7" max="7" width="11.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="62"/>
+    <col min="3" max="3" width="9.109375" style="62" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="62" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="62" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="62"/>
+    <col min="7" max="7" width="11.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
@@ -10739,11 +10793,11 @@
       <c r="D1" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="259" t="s">
+      <c r="E1" s="260" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
@@ -10757,9 +10811,9 @@
       <c r="D2" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E2" s="259"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E2" s="260"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
@@ -10773,9 +10827,9 @@
       <c r="D3" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E3" s="259"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E3" s="260"/>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
@@ -10789,9 +10843,9 @@
       <c r="D4" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E4" s="259"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E4" s="260"/>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
@@ -10805,9 +10859,9 @@
       <c r="D5" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="259"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E5" s="260"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
         <v>83</v>
       </c>
@@ -10821,9 +10875,9 @@
       <c r="D6" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="E6" s="259"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="260"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="89" t="s">
         <v>84</v>
       </c>
@@ -10837,7 +10891,7 @@
       <c r="D7" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="E7" s="260"/>
+      <c r="E7" s="261"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10850,23 +10904,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" style="62" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="62" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="62"/>
-    <col min="4" max="4" width="79.7109375" style="62" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="62" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="1" width="37.6640625" style="62" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="62" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="79.6640625" style="62" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>188</v>
       </c>
@@ -10881,7 +10936,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>189</v>
       </c>
@@ -10896,7 +10951,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>190</v>
       </c>
@@ -10911,7 +10966,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>191</v>
       </c>
@@ -10926,7 +10981,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>192</v>
       </c>
@@ -10940,7 +10995,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="138" t="s">
         <v>220</v>
       </c>
@@ -10954,7 +11009,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>194</v>
       </c>
@@ -10969,7 +11024,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>270</v>
       </c>
@@ -10984,7 +11039,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="219" t="s">
         <v>283</v>
       </c>
@@ -10998,7 +11053,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="240" t="s">
         <v>286</v>
       </c>
@@ -11012,7 +11067,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>195</v>
       </c>
@@ -11027,7 +11082,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>117</v>
       </c>
@@ -11041,7 +11096,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>205</v>
       </c>
@@ -11055,7 +11110,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="138" t="s">
         <v>207</v>
       </c>
@@ -11069,7 +11124,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="77" t="s">
         <v>208</v>
       </c>
@@ -11083,7 +11138,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A16" s="108" t="s">
         <v>193</v>
       </c>
@@ -11098,54 +11153,54 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="69"/>
       <c r="B17" s="94"/>
       <c r="C17" s="69"/>
       <c r="D17" s="69"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="148"/>
       <c r="C18" s="232"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C19" s="94"/>
       <c r="D19" s="69"/>
       <c r="E19" s="69"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" s="69"/>
       <c r="D20" s="94"/>
       <c r="E20" s="69"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="231"/>
       <c r="C21" s="69"/>
       <c r="D21" s="69"/>
       <c r="E21" s="94"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="234"/>
       <c r="C22" s="235"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A15:D15">
-    <cfRule type="expression" dxfId="71" priority="5">
+    <cfRule type="expression" dxfId="75" priority="5">
       <formula>$B$14&lt;&gt;"mechanistic"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:D16">
-    <cfRule type="expression" dxfId="70" priority="4">
+    <cfRule type="expression" dxfId="74" priority="4">
       <formula>$B$14&lt;&gt;"naive"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D10">
-    <cfRule type="expression" dxfId="69" priority="2">
+    <cfRule type="expression" dxfId="73" priority="2">
       <formula>OR($B$6 = "granule", $B$6 = "mature granule")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:D8">
-    <cfRule type="expression" dxfId="68" priority="3">
+    <cfRule type="expression" dxfId="72" priority="3">
       <formula>$B$6 ="suspension"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11167,19 +11222,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>218</v>
       </c>
@@ -11193,7 +11249,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>221</v>
       </c>
@@ -11207,7 +11263,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>187</v>
       </c>
@@ -11221,7 +11277,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>252</v>
       </c>
@@ -11235,7 +11291,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A5" s="108" t="s">
         <v>224</v>
       </c>
@@ -11249,7 +11305,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>225</v>
       </c>
@@ -11264,7 +11320,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>212</v>
       </c>
@@ -11278,7 +11334,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
         <v>213</v>
       </c>
@@ -11292,7 +11348,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>215</v>
       </c>
@@ -11306,7 +11362,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A10" s="108" t="s">
         <v>227</v>
       </c>
@@ -11320,7 +11376,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>255</v>
       </c>
@@ -11334,7 +11390,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>254</v>
       </c>
@@ -11350,17 +11406,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:D4">
-    <cfRule type="expression" dxfId="67" priority="3">
+    <cfRule type="expression" dxfId="71" priority="3">
       <formula>$B$2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:D12">
-    <cfRule type="expression" dxfId="66" priority="2">
+    <cfRule type="expression" dxfId="70" priority="2">
       <formula>$B$11=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:D5">
-    <cfRule type="expression" dxfId="65" priority="1">
+    <cfRule type="expression" dxfId="69" priority="1">
       <formula>$B$2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11382,21 +11438,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="62"/>
-    <col min="4" max="4" width="4.42578125" style="62" customWidth="1"/>
-    <col min="5" max="5" width="62.5703125" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="62"/>
+    <col min="1" max="3" width="9.109375" style="62"/>
+    <col min="4" max="4" width="4.44140625" style="62" customWidth="1"/>
+    <col min="5" max="5" width="62.5546875" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="62"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
         <v>74</v>
       </c>
@@ -11410,7 +11467,7 @@
       <c r="D1" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="261" t="s">
+      <c r="E1" s="262" t="s">
         <v>230</v>
       </c>
       <c r="F1" s="69"/>
@@ -11419,7 +11476,7 @@
       <c r="I1" s="69"/>
       <c r="J1" s="69"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
@@ -11433,19 +11490,19 @@
       <c r="D2" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="261"/>
+      <c r="E2" s="262"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
       <c r="J2" s="69"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="131">
-        <f t="shared" ref="B3" si="0">500*10^(-6)</f>
+        <f>500*10^(-6)</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="C3" s="90" t="s">
@@ -11454,39 +11511,39 @@
       <c r="D3" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="261"/>
+      <c r="E3" s="262"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
       <c r="I3" s="69"/>
       <c r="J3" s="69"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="131">
-        <f>50*10^(-6)</f>
-        <v>4.9999999999999996E-5</v>
+        <f>1*10^(-6)</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>87</v>
       </c>
       <c r="D4" s="143" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="261"/>
+        <v>90</v>
+      </c>
+      <c r="E4" s="262"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
       <c r="I4" s="69"/>
       <c r="J4" s="69"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="131">
+      <c r="B5" s="118">
         <v>1E-3</v>
       </c>
       <c r="C5" s="90" t="s">
@@ -11495,14 +11552,14 @@
       <c r="D5" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="261"/>
+      <c r="E5" s="262"/>
       <c r="F5" s="94"/>
       <c r="G5" s="69"/>
       <c r="H5" s="69"/>
       <c r="I5" s="69"/>
       <c r="J5" s="69"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>83</v>
       </c>
@@ -11516,14 +11573,14 @@
       <c r="D6" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="261"/>
+      <c r="E6" s="262"/>
       <c r="F6" s="94"/>
       <c r="G6" s="69"/>
       <c r="H6" s="69"/>
       <c r="I6" s="69"/>
       <c r="J6" s="69"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
         <v>84</v>
       </c>
@@ -11537,14 +11594,14 @@
       <c r="D7" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="261"/>
+      <c r="E7" s="262"/>
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
       <c r="H7" s="69"/>
       <c r="I7" s="69"/>
       <c r="J7" s="69"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="69"/>
       <c r="B13" s="69"/>
       <c r="C13" s="69"/>
@@ -11556,7 +11613,7 @@
       <c r="I13" s="69"/>
       <c r="J13" s="70"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="69"/>
       <c r="B16" s="69"/>
       <c r="C16" s="69"/>

</xml_diff>